<commit_message>
Update User story_Team genesis.xlsx
</commit_message>
<xml_diff>
--- a/Requirements/User story_Team genesis.xlsx
+++ b/Requirements/User story_Team genesis.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25207"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC0F714B-5986-49E0-9DCD-CC654C6DC384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69F1EBF7-5A5C-4D53-99A4-F1B780CD5039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="279">
   <si>
     <t>Modules and Attributes</t>
   </si>
@@ -310,9 +310,6 @@
     <t>Layout Should be same form first to last</t>
   </si>
   <si>
-    <t>Change list to grid</t>
-  </si>
-  <si>
     <t>Implement - back to same page</t>
   </si>
   <si>
@@ -344,6 +341,27 @@
   </si>
   <si>
     <t>Get reporting person in dropbox (as list)</t>
+  </si>
+  <si>
+    <t>Add last approved date</t>
+  </si>
+  <si>
+    <t>Add save and next</t>
+  </si>
+  <si>
+    <t>Add box for profile image</t>
+  </si>
+  <si>
+    <t>Add delete and edit for all drop down added details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design social media </t>
+  </si>
+  <si>
+    <t>Add text based filter for project</t>
+  </si>
+  <si>
+    <t>Entity Model Normalization</t>
   </si>
   <si>
     <t>Team Genesis - Profile Management Project</t>
@@ -475,6 +493,9 @@
     <t>So other can see the user profile</t>
   </si>
   <si>
+    <t>Reporting person should able to accept or reject the user profile</t>
+  </si>
+  <si>
     <t xml:space="preserve">I should be able to logout(reused) to </t>
   </si>
   <si>
@@ -496,7 +517,7 @@
     <t>So I can maintain the data upto date</t>
   </si>
   <si>
-    <t xml:space="preserve">Admin should have the privilege to add or change the master data()			</t>
+    <t xml:space="preserve">Admin should have the privilege to add or change the master data(Designation,College,Experience,Technology)			</t>
   </si>
   <si>
     <t xml:space="preserve">I should be able to add HR Partner </t>
@@ -517,9 +538,6 @@
     <t>I should be able to logout(reused)</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>HR Partner</t>
   </si>
   <si>
@@ -537,6 +555,9 @@
   </si>
   <si>
     <t xml:space="preserve">So They can approves user profile </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I should able to assign reporting person  </t>
   </si>
   <si>
     <t>Entity  model</t>
@@ -1251,20 +1272,20 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 2">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DC57BCE-A5E6-2D20-710D-0D77E261F4D4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A326E9F-6AAC-452D-09EB-D248E335FEEB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1280,8 +1301,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4010025" y="657225"/>
-          <a:ext cx="5857875" cy="6353175"/>
+          <a:off x="4010025" y="695325"/>
+          <a:ext cx="11811000" cy="10915650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -34340,9 +34361,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
@@ -34630,44 +34651,77 @@
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="3:3" ht="15.75" customHeight="1">
+    <row r="49" spans="1:3" ht="15.75" customHeight="1">
       <c r="C49" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="3:3" ht="15.75" customHeight="1">
+    <row r="50" spans="1:3" ht="15.75" customHeight="1">
       <c r="C50" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="3:3" ht="15.75" customHeight="1">
+    <row r="51" spans="1:3" ht="15.75" customHeight="1">
       <c r="C51" s="7" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="3:3" ht="15.75" customHeight="1">
+    <row r="52" spans="1:3" ht="15.75" customHeight="1">
       <c r="C52" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="3:3" ht="15.75" customHeight="1">
+    <row r="53" spans="1:3" ht="15.75" customHeight="1">
       <c r="C53" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="3:3" ht="15.75" customHeight="1">
+    <row r="54" spans="1:3" ht="15.75" customHeight="1">
       <c r="C54" s="7" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="3:3" ht="15.75" customHeight="1">
+    <row r="55" spans="1:3" ht="15.75" customHeight="1">
       <c r="C55" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="3:3" ht="15.75" customHeight="1">
-      <c r="C56" s="7" t="s">
+    <row r="58" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A58" s="9">
+        <v>44660</v>
+      </c>
+      <c r="C58" s="7" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C59" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C60" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C61" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C62" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C63" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="15.75" customHeight="1">
+      <c r="C64" s="7" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -34679,8 +34733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99455432-5260-4250-8176-F630DA6BD87E}">
   <dimension ref="A5:G48"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -34690,12 +34744,12 @@
     <col min="4" max="4" width="14" style="15" customWidth="1"/>
     <col min="5" max="5" width="93.5703125" customWidth="1"/>
     <col min="6" max="6" width="58.85546875" customWidth="1"/>
-    <col min="7" max="7" width="80.28515625" customWidth="1"/>
+    <col min="7" max="7" width="98" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5">
       <c r="E5" s="15" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -34703,27 +34757,27 @@
     </row>
     <row r="10" spans="1:5">
       <c r="E10" s="15" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="15" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="G18" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="2:7">
@@ -34731,31 +34785,31 @@
         <v>1</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D19" s="15">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="F19" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="2:7" ht="38.25">
+    <row r="20" spans="2:7" ht="36">
       <c r="D20" s="15">
         <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="F20" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="G20" s="40" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="39.75" customHeight="1">
@@ -34763,13 +34817,13 @@
         <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="F21" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="G21" s="40" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="12.75" customHeight="1">
@@ -34777,13 +34831,13 @@
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F22" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="2:7">
@@ -34791,13 +34845,13 @@
         <v>5</v>
       </c>
       <c r="E23" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="F23" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="2:7">
@@ -34805,10 +34859,10 @@
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="F24" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="G24" s="12"/>
     </row>
@@ -34824,16 +34878,16 @@
         <v>2</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D27" s="15">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="F27" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G27" s="12"/>
     </row>
@@ -34842,10 +34896,10 @@
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="F28" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G28" s="12"/>
     </row>
@@ -34854,13 +34908,13 @@
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="F29" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="2:7">
@@ -34868,13 +34922,13 @@
         <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="F30" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="2:7">
@@ -34882,13 +34936,13 @@
         <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="F31" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="2:7">
@@ -34896,13 +34950,13 @@
         <v>6</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="G32" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="2:7">
@@ -34910,13 +34964,13 @@
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="F33" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="2:7">
@@ -34924,22 +34978,24 @@
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="F34" t="s">
-        <v>144</v>
-      </c>
-      <c r="G34" s="12"/>
+        <v>150</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="35" spans="2:7">
       <c r="D35" s="15">
         <v>9</v>
       </c>
       <c r="E35" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="F35" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="G35" s="12"/>
     </row>
@@ -34954,16 +35010,16 @@
         <v>3</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D37" s="15">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="F37" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G37" s="12"/>
     </row>
@@ -34973,10 +35029,10 @@
         <v>2</v>
       </c>
       <c r="E38" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="F38" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="G38" s="12"/>
     </row>
@@ -34985,13 +35041,13 @@
         <v>3</v>
       </c>
       <c r="E39" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="F39" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="2:7">
@@ -34999,13 +35055,13 @@
         <v>4</v>
       </c>
       <c r="E40" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="F40" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="2:7">
@@ -35013,10 +35069,10 @@
         <v>5</v>
       </c>
       <c r="E41" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="F41" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="G41" s="12"/>
     </row>
@@ -35025,18 +35081,15 @@
         <v>6</v>
       </c>
       <c r="E42" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="F42" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="G42" s="12"/>
     </row>
     <row r="43" spans="2:7" ht="15">
       <c r="E43" s="4"/>
-      <c r="F43" t="s">
-        <v>159</v>
-      </c>
       <c r="G43" s="12"/>
     </row>
     <row r="44" spans="2:7">
@@ -35044,16 +35097,16 @@
         <v>4</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D44" s="15">
         <v>1</v>
       </c>
       <c r="E44" s="38" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="F44" s="39" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="G44" s="12"/>
     </row>
@@ -35062,13 +35115,13 @@
         <v>2</v>
       </c>
       <c r="E45" s="33" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="F45" s="33" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="G45" s="40" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="2:7">
@@ -35076,22 +35129,24 @@
         <v>3</v>
       </c>
       <c r="E46" s="33" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="F46" t="s">
-        <v>165</v>
-      </c>
-      <c r="G46" s="12"/>
+        <v>171</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="47" spans="2:7">
       <c r="D47" s="15">
         <v>4</v>
       </c>
       <c r="E47" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="F47" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="G47" s="12"/>
     </row>
@@ -35112,13 +35167,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB4FBD0-7C1E-4BC2-A19C-4CB4A94AE885}">
   <dimension ref="L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AA45" sqref="AA45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="2" spans="12:12">
       <c r="L2" s="13" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -35131,7 +35188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79905DE3-DAB3-4C6E-84FE-24BF5F973564}">
   <dimension ref="C1:K603"/>
   <sheetViews>
-    <sheetView topLeftCell="S107" workbookViewId="0">
+    <sheetView topLeftCell="S137" workbookViewId="0">
       <selection activeCell="AE151" sqref="AE151"/>
     </sheetView>
   </sheetViews>
@@ -35139,28 +35196,28 @@
   <sheetData>
     <row r="1" spans="3:10" ht="23.25">
       <c r="J1" s="20" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="3:10" ht="20.25">
       <c r="C4" s="19" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D4" s="13"/>
     </row>
     <row r="6" spans="3:10" ht="20.25">
       <c r="D6" s="18" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="4:4" ht="20.25">
       <c r="D21" s="18" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="4:8" ht="20.25">
       <c r="D33" s="21" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="4:8">
@@ -35168,34 +35225,34 @@
     </row>
     <row r="46" spans="4:8" ht="20.25">
       <c r="D46" s="18" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" spans="3:4" ht="20.25">
       <c r="C59" s="19" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="D59" s="18"/>
     </row>
     <row r="61" spans="3:4" ht="20.25">
       <c r="D61" s="18" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
     </row>
     <row r="74" spans="4:5" ht="20.25">
       <c r="D74" s="18" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E74" s="18"/>
     </row>
     <row r="85" spans="4:4" ht="20.25">
       <c r="D85" s="18" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="296" spans="3:5" ht="18">
       <c r="C296" s="16" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="D296" s="16"/>
       <c r="E296" s="16"/>
@@ -35215,8 +35272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF61F9D4-CE67-4B1A-BDEF-73A765CC6053}">
   <dimension ref="A1:Q88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -35227,7 +35284,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15">
       <c r="A1" s="37" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -35235,170 +35292,170 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="F3" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B5" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="B6" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="B9" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B10" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B12" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15">
       <c r="A16" s="37" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B17" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B19" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="B20" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B22" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B24" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15">
       <c r="A27" s="37" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="13" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B29" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B31" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:17">
       <c r="B33" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
     </row>
     <row r="35" spans="1:17">
       <c r="A35" s="13" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
     </row>
     <row r="36" spans="1:17">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B36" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:17">
       <c r="A38" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B38" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="39" spans="1:17">
       <c r="B39" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:17">
       <c r="B40" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="I40" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:17">
       <c r="I41" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="1:17">
@@ -35406,153 +35463,153 @@
     </row>
     <row r="45" spans="1:17">
       <c r="A45" s="13" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="46" spans="1:17">
       <c r="A46" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:17">
       <c r="A48" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B48" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="B49" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15">
       <c r="A51" s="37" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B52" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B54" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15">
       <c r="A64" s="37" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="13" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B68" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="B69" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="13" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B74" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B76" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="B77" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="13" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B82" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="B83" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15">
       <c r="A85" s="37" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B86" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B88" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -35564,8 +35621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDCE65D9-B3F5-4A6F-B0B3-3A621DFF1ACB}">
   <dimension ref="A3:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -35575,7 +35632,7 @@
   <sheetData>
     <row r="3" spans="1:2">
       <c r="B3" s="13" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -35583,7 +35640,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -35591,7 +35648,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -35599,7 +35656,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -35607,7 +35664,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="B10" s="13" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -35615,7 +35672,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -35623,7 +35680,7 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -35631,7 +35688,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -35639,7 +35696,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -35647,7 +35704,7 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -35655,7 +35712,7 @@
         <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -35663,7 +35720,7 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -35671,7 +35728,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -35679,7 +35736,7 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -35687,7 +35744,7 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -35700,7 +35757,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -35716,10 +35773,10 @@
     <row r="1" spans="1:3">
       <c r="A1" s="25"/>
       <c r="B1" s="26" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C1" s="27" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -35729,47 +35786,47 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="23" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="23"/>
       <c r="B4" s="24" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="23"/>
       <c r="B5" s="24" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="23"/>
       <c r="B6" s="24" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="23"/>
       <c r="B7" s="24"/>
       <c r="C7" s="23" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -35824,10 +35881,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="23" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="C18" s="23" t="s">
         <v>4</v>
@@ -35836,31 +35893,31 @@
     <row r="19" spans="1:4">
       <c r="A19" s="23"/>
       <c r="B19" s="24" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="23"/>
       <c r="B20" s="24" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="D20" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="23"/>
       <c r="B21" s="24" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -35894,128 +35951,128 @@
   <sheetData>
     <row r="3" spans="1:15" ht="20.25">
       <c r="L3" s="18" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="B9" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="O9" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="B15" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="B17" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="O17" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="B19" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="B21" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="B23" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="B25" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="O25" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
     </row>
     <row r="32" spans="1:15">
       <c r="O32" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
     </row>
     <row r="39" spans="15:15">
       <c r="O39" s="33" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
     </row>
     <row r="47" spans="15:15">
       <c r="O47" s="33" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
     </row>
     <row r="55" spans="15:15">
       <c r="O55" s="33" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
     </row>
     <row r="63" spans="15:15">
       <c r="O63" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
     </row>
     <row r="71" spans="15:15">
       <c r="O71" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
     </row>
     <row r="79" spans="15:15">
       <c r="O79" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated MOM and Entitymodel with operations
</commit_message>
<xml_diff>
--- a/Requirements/User story_Team genesis.xlsx
+++ b/Requirements/User story_Team genesis.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25217"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A594B406-9A8B-4971-9144-4D01A038487B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C969031E-9D27-42D1-B332-57DAD3C01E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="4" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="481">
   <si>
     <t>Modules and Attributes</t>
   </si>
@@ -437,6 +437,18 @@
   </si>
   <si>
     <t>Prepare a sample control and showcase within saturday</t>
+  </si>
+  <si>
+    <t>Seperate services for user and profile</t>
+  </si>
+  <si>
+    <t>Refer personal details id in all profile related tables</t>
+  </si>
+  <si>
+    <t>Find services and operations from prototype</t>
+  </si>
+  <si>
+    <t>Design layered system architechture</t>
   </si>
   <si>
     <t>Team Genesis - Profile Management Project</t>
@@ -1633,7 +1645,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1666,12 +1678,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF8CBAD"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD0CECE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1683,7 +1689,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1956,19 +1962,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -2116,12 +2109,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2185,15 +2262,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2203,8 +2271,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2220,11 +2288,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2240,6 +2308,63 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="38" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2252,10 +2377,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2264,7 +2389,7 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2283,48 +2408,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2561,23 +2644,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>127</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 3">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9CA5775-F552-27DF-4C3F-441CF1239D95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1D0FC45-DFA6-061C-3E24-A84984253001}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{C9CA5775-F552-27DF-4C3F-441CF1239D95}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2593,8 +2679,55 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2133600" y="2828925"/>
-          <a:ext cx="10144125" cy="17830800"/>
+          <a:off x="3038475" y="342900"/>
+          <a:ext cx="9648825" cy="16202025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18E3D19E-8A76-2461-42CE-A237A3244498}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D1D0FC45-DFA6-061C-3E24-A84984253001}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2409825" y="23764875"/>
+          <a:ext cx="10363200" cy="16840200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -35655,10 +35788,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F98" sqref="F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -35669,24 +35802,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="35.25" customHeight="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="86" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="26" customFormat="1" ht="12.75">
-      <c r="A2" s="89">
+      <c r="A2" s="87">
         <v>44653</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="88" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="89" t="s">
         <v>43</v>
       </c>
     </row>
@@ -35701,600 +35834,630 @@
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="12.75">
-      <c r="A5" s="90">
+      <c r="A5" s="71">
         <v>44655</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="92" t="s">
+      <c r="C5" s="73" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="12.75">
-      <c r="A6" s="93"/>
+      <c r="A6" s="74"/>
       <c r="B6" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="94" t="s">
+      <c r="C6" s="75" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A7" s="93"/>
+      <c r="A7" s="74"/>
       <c r="B7" s="24"/>
-      <c r="C7" s="95" t="s">
+      <c r="C7" s="76" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A8" s="96"/>
-      <c r="B8" s="97"/>
-      <c r="C8" s="98" t="s">
+      <c r="A8" s="77"/>
+      <c r="B8" s="78"/>
+      <c r="C8" s="79" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A10" s="99">
+      <c r="A10" s="80">
         <v>44656</v>
       </c>
-      <c r="B10" s="100" t="s">
+      <c r="B10" s="81" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="101" t="s">
+      <c r="C10" s="82" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A11" s="93"/>
+      <c r="A11" s="74"/>
       <c r="B11" s="24"/>
-      <c r="C11" s="95" t="s">
+      <c r="C11" s="76" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A12" s="93"/>
+      <c r="A12" s="74"/>
       <c r="B12" s="24"/>
-      <c r="C12" s="95" t="s">
+      <c r="C12" s="76" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A13" s="93"/>
+      <c r="A13" s="74"/>
       <c r="B13" s="24"/>
-      <c r="C13" s="95" t="s">
+      <c r="C13" s="76" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A14" s="93"/>
+      <c r="A14" s="74"/>
       <c r="B14" s="24"/>
-      <c r="C14" s="95" t="s">
+      <c r="C14" s="76" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A15" s="96"/>
-      <c r="B15" s="97"/>
-      <c r="C15" s="98" t="s">
+      <c r="A15" s="77"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="79" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A17" s="99">
+      <c r="A17" s="80">
         <v>44657</v>
       </c>
-      <c r="B17" s="100" t="s">
+      <c r="B17" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="101" t="s">
+      <c r="C17" s="82" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A18" s="93"/>
+      <c r="A18" s="74"/>
       <c r="B18" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="95" t="s">
+      <c r="C18" s="76" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A19" s="93"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="24"/>
-      <c r="C19" s="95" t="s">
+      <c r="C19" s="76" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A20" s="93"/>
+      <c r="A20" s="74"/>
       <c r="B20" s="24"/>
-      <c r="C20" s="95" t="s">
+      <c r="C20" s="76" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="93"/>
+      <c r="A21" s="74"/>
       <c r="B21" s="24"/>
-      <c r="C21" s="95" t="s">
+      <c r="C21" s="76" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="93"/>
+      <c r="A22" s="74"/>
       <c r="B22" s="24"/>
-      <c r="C22" s="95" t="s">
+      <c r="C22" s="76" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="93"/>
+      <c r="A23" s="74"/>
       <c r="B23" s="24"/>
-      <c r="C23" s="95" t="s">
+      <c r="C23" s="76" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="93"/>
+      <c r="A24" s="74"/>
       <c r="B24" s="24"/>
-      <c r="C24" s="95" t="s">
+      <c r="C24" s="76" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="93"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="24"/>
-      <c r="C25" s="95" t="s">
+      <c r="C25" s="76" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A26" s="93"/>
+      <c r="A26" s="74"/>
       <c r="B26" s="24"/>
-      <c r="C26" s="95" t="s">
+      <c r="C26" s="76" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A27" s="93"/>
+      <c r="A27" s="74"/>
       <c r="B27" s="24"/>
-      <c r="C27" s="95" t="s">
+      <c r="C27" s="76" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A28" s="96"/>
-      <c r="B28" s="97"/>
-      <c r="C28" s="98" t="s">
+      <c r="A28" s="77"/>
+      <c r="B28" s="78"/>
+      <c r="C28" s="79" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A30" s="99">
+      <c r="A30" s="80">
         <v>44658</v>
       </c>
-      <c r="B30" s="100" t="s">
+      <c r="B30" s="81" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="101" t="s">
+      <c r="C30" s="82" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A31" s="93"/>
+      <c r="A31" s="74"/>
       <c r="B31" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="95" t="s">
+      <c r="C31" s="76" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A32" s="93"/>
+      <c r="A32" s="74"/>
       <c r="B32" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="95" t="s">
+      <c r="C32" s="76" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A33" s="93"/>
+      <c r="A33" s="74"/>
       <c r="B33" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="95" t="s">
+      <c r="C33" s="76" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A34" s="93"/>
+      <c r="A34" s="74"/>
       <c r="B34" s="24"/>
-      <c r="C34" s="95" t="s">
+      <c r="C34" s="76" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A35" s="93"/>
+      <c r="A35" s="74"/>
       <c r="B35" s="24"/>
-      <c r="C35" s="95" t="s">
+      <c r="C35" s="76" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A36" s="93"/>
+      <c r="A36" s="74"/>
       <c r="B36" s="24"/>
-      <c r="C36" s="95" t="s">
+      <c r="C36" s="76" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A37" s="93"/>
+      <c r="A37" s="74"/>
       <c r="B37" s="24"/>
-      <c r="C37" s="95" t="s">
+      <c r="C37" s="76" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A38" s="93"/>
+      <c r="A38" s="74"/>
       <c r="B38" s="24"/>
-      <c r="C38" s="95" t="s">
+      <c r="C38" s="76" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A39" s="93"/>
+      <c r="A39" s="74"/>
       <c r="B39" s="24"/>
-      <c r="C39" s="95" t="s">
+      <c r="C39" s="76" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A40" s="93"/>
+      <c r="A40" s="74"/>
       <c r="B40" s="24"/>
-      <c r="C40" s="95" t="s">
+      <c r="C40" s="76" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A41" s="93"/>
+      <c r="A41" s="74"/>
       <c r="B41" s="24"/>
-      <c r="C41" s="95" t="s">
+      <c r="C41" s="76" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A42" s="93"/>
+      <c r="A42" s="74"/>
       <c r="B42" s="24"/>
-      <c r="C42" s="95" t="s">
+      <c r="C42" s="76" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A43" s="96"/>
-      <c r="B43" s="97"/>
-      <c r="C43" s="98" t="s">
+      <c r="A43" s="77"/>
+      <c r="B43" s="78"/>
+      <c r="C43" s="79" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A45" s="99">
+      <c r="A45" s="80">
         <v>44659</v>
       </c>
-      <c r="B45" s="102" t="s">
+      <c r="B45" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="101" t="s">
+      <c r="C45" s="82" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A46" s="93"/>
+      <c r="A46" s="74"/>
       <c r="B46" s="24"/>
-      <c r="C46" s="95" t="s">
+      <c r="C46" s="76" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A47" s="93"/>
+      <c r="A47" s="74"/>
       <c r="B47" s="24"/>
-      <c r="C47" s="95" t="s">
+      <c r="C47" s="76" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A48" s="93"/>
+      <c r="A48" s="74"/>
       <c r="B48" s="24"/>
-      <c r="C48" s="95" t="s">
+      <c r="C48" s="76" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A49" s="93"/>
+      <c r="A49" s="74"/>
       <c r="B49" s="24"/>
-      <c r="C49" s="95" t="s">
+      <c r="C49" s="76" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A50" s="93"/>
+      <c r="A50" s="74"/>
       <c r="B50" s="24"/>
-      <c r="C50" s="95" t="s">
+      <c r="C50" s="76" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A51" s="93"/>
+      <c r="A51" s="74"/>
       <c r="B51" s="24"/>
-      <c r="C51" s="95" t="s">
+      <c r="C51" s="76" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A52" s="93"/>
+      <c r="A52" s="74"/>
       <c r="B52" s="24"/>
-      <c r="C52" s="95" t="s">
+      <c r="C52" s="76" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A53" s="93"/>
+      <c r="A53" s="74"/>
       <c r="B53" s="24"/>
-      <c r="C53" s="95" t="s">
+      <c r="C53" s="76" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A54" s="93"/>
+      <c r="A54" s="74"/>
       <c r="B54" s="24"/>
-      <c r="C54" s="95" t="s">
+      <c r="C54" s="76" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A55" s="93"/>
+      <c r="A55" s="74"/>
       <c r="B55" s="24"/>
-      <c r="C55" s="95" t="s">
+      <c r="C55" s="76" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A56" s="93"/>
+      <c r="A56" s="74"/>
       <c r="B56" s="24"/>
-      <c r="C56" s="95" t="s">
+      <c r="C56" s="76" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A57" s="96"/>
-      <c r="B57" s="97"/>
-      <c r="C57" s="98" t="s">
+      <c r="A57" s="77"/>
+      <c r="B57" s="78"/>
+      <c r="C57" s="79" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A60" s="99">
+      <c r="A60" s="80">
         <v>44660</v>
       </c>
-      <c r="B60" s="100"/>
-      <c r="C60" s="101" t="s">
+      <c r="B60" s="81"/>
+      <c r="C60" s="82" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A61" s="93"/>
+      <c r="A61" s="74"/>
       <c r="B61" s="24"/>
-      <c r="C61" s="95" t="s">
+      <c r="C61" s="76" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A62" s="93"/>
+      <c r="A62" s="74"/>
       <c r="B62" s="24"/>
-      <c r="C62" s="95" t="s">
+      <c r="C62" s="76" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A63" s="93"/>
+      <c r="A63" s="74"/>
       <c r="B63" s="24"/>
-      <c r="C63" s="95" t="s">
+      <c r="C63" s="76" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A64" s="93"/>
+      <c r="A64" s="74"/>
       <c r="B64" s="24"/>
-      <c r="C64" s="95" t="s">
+      <c r="C64" s="76" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A65" s="93"/>
+      <c r="A65" s="74"/>
       <c r="B65" s="24"/>
-      <c r="C65" s="95" t="s">
+      <c r="C65" s="76" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A66" s="96"/>
-      <c r="B66" s="97"/>
-      <c r="C66" s="98" t="s">
+      <c r="A66" s="77"/>
+      <c r="B66" s="78"/>
+      <c r="C66" s="79" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A68" s="99">
+      <c r="A68" s="80">
         <v>44662</v>
       </c>
-      <c r="B68" s="100" t="s">
+      <c r="B68" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="C68" s="101" t="s">
+      <c r="C68" s="82" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A69" s="93"/>
+      <c r="A69" s="74"/>
       <c r="B69" s="24"/>
-      <c r="C69" s="95" t="s">
+      <c r="C69" s="76" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A70" s="93"/>
+      <c r="A70" s="74"/>
       <c r="B70" s="24"/>
-      <c r="C70" s="95" t="s">
+      <c r="C70" s="76" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A71" s="93"/>
+      <c r="A71" s="74"/>
       <c r="B71" s="24"/>
-      <c r="C71" s="95" t="s">
+      <c r="C71" s="76" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A72" s="93"/>
+      <c r="A72" s="74"/>
       <c r="B72" s="24"/>
-      <c r="C72" s="95" t="s">
+      <c r="C72" s="76" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A73" s="93"/>
+      <c r="A73" s="74"/>
       <c r="B73" s="24"/>
-      <c r="C73" s="95" t="s">
+      <c r="C73" s="76" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A74" s="93"/>
+      <c r="A74" s="74"/>
       <c r="B74" s="24"/>
-      <c r="C74" s="95" t="s">
+      <c r="C74" s="76" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A75" s="93"/>
+      <c r="A75" s="74"/>
       <c r="B75" s="24"/>
-      <c r="C75" s="95" t="s">
+      <c r="C75" s="76" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A76" s="93"/>
+      <c r="A76" s="74"/>
       <c r="B76" s="24"/>
-      <c r="C76" s="95" t="s">
+      <c r="C76" s="76" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A77" s="93"/>
+      <c r="A77" s="74"/>
       <c r="B77" s="24"/>
-      <c r="C77" s="95" t="s">
+      <c r="C77" s="76" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A78" s="96"/>
-      <c r="B78" s="97"/>
-      <c r="C78" s="98" t="s">
+      <c r="A78" s="77"/>
+      <c r="B78" s="78"/>
+      <c r="C78" s="79" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A80" s="99">
+      <c r="A80" s="80">
         <v>44663</v>
       </c>
-      <c r="B80" s="100"/>
-      <c r="C80" s="101" t="s">
+      <c r="B80" s="81"/>
+      <c r="C80" s="82" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A81" s="93"/>
+      <c r="A81" s="74"/>
       <c r="B81" s="24"/>
-      <c r="C81" s="95" t="s">
+      <c r="C81" s="76" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A82" s="93"/>
+      <c r="A82" s="74"/>
       <c r="B82" s="24"/>
-      <c r="C82" s="95" t="s">
+      <c r="C82" s="76" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A83" s="93"/>
+      <c r="A83" s="74"/>
       <c r="B83" s="24"/>
-      <c r="C83" s="95" t="s">
+      <c r="C83" s="76" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A84" s="96"/>
-      <c r="B84" s="97"/>
-      <c r="C84" s="98" t="s">
+      <c r="A84" s="77"/>
+      <c r="B84" s="78"/>
+      <c r="C84" s="79" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A86" s="99">
+      <c r="A86" s="80">
         <v>44664</v>
       </c>
-      <c r="B86" s="100" t="s">
+      <c r="B86" s="81" t="s">
         <v>126</v>
       </c>
-      <c r="C86" s="101" t="s">
+      <c r="C86" s="82" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A87" s="93"/>
+      <c r="A87" s="74"/>
       <c r="B87" s="24"/>
-      <c r="C87" s="95" t="s">
+      <c r="C87" s="76" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A88" s="93"/>
+      <c r="A88" s="74"/>
       <c r="B88" s="24"/>
-      <c r="C88" s="95" t="s">
+      <c r="C88" s="76" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A89" s="96"/>
-      <c r="B89" s="97"/>
-      <c r="C89" s="98" t="s">
+      <c r="A89" s="77"/>
+      <c r="B89" s="78"/>
+      <c r="C89" s="79" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A91" s="99">
+      <c r="A91" s="80">
         <v>44671</v>
       </c>
-      <c r="B91" s="100"/>
-      <c r="C91" s="101" t="s">
+      <c r="B91" s="81"/>
+      <c r="C91" s="82" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A92" s="93"/>
+      <c r="A92" s="74"/>
       <c r="B92" s="24"/>
-      <c r="C92" s="95" t="s">
+      <c r="C92" s="76" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A93" s="96"/>
-      <c r="B93" s="97"/>
-      <c r="C93" s="98" t="s">
+      <c r="A93" s="77"/>
+      <c r="B93" s="78"/>
+      <c r="C93" s="79" t="s">
         <v>133</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A95" s="80">
+        <v>44672</v>
+      </c>
+      <c r="B95" s="81"/>
+      <c r="C95" s="82" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A96" s="74"/>
+      <c r="B96" s="24"/>
+      <c r="C96" s="76" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A97" s="74"/>
+      <c r="B97" s="24"/>
+      <c r="C97" s="76" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A98" s="77"/>
+      <c r="B98" s="78"/>
+      <c r="C98" s="79" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -36324,7 +36487,7 @@
   <sheetData>
     <row r="5" spans="1:5">
       <c r="E5" s="8" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -36332,726 +36495,726 @@
     </row>
     <row r="10" spans="1:5">
       <c r="E10" s="8" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="2:9">
-      <c r="B18" s="56" t="s">
-        <v>136</v>
-      </c>
-      <c r="C18" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="D18" s="56" t="s">
-        <v>138</v>
-      </c>
-      <c r="E18" s="56" t="s">
-        <v>139</v>
-      </c>
-      <c r="F18" s="56" t="s">
+      <c r="B18" s="53" t="s">
         <v>140</v>
       </c>
+      <c r="C18" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="D18" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="E18" s="53" t="s">
+        <v>143</v>
+      </c>
+      <c r="F18" s="53" t="s">
+        <v>144</v>
+      </c>
       <c r="G18" s="15" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="51">
-      <c r="B19" s="56">
+      <c r="B19" s="53">
         <v>1</v>
       </c>
-      <c r="C19" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="D19" s="56">
+      <c r="C19" s="53" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="53">
         <v>1</v>
       </c>
-      <c r="E19" s="57" t="s">
-        <v>145</v>
-      </c>
-      <c r="F19" s="57" t="s">
-        <v>146</v>
-      </c>
-      <c r="G19" s="58" t="s">
-        <v>147</v>
-      </c>
-      <c r="H19" s="58" t="s">
-        <v>148</v>
-      </c>
-      <c r="I19" s="59" t="s">
+      <c r="E19" s="54" t="s">
         <v>149</v>
+      </c>
+      <c r="F19" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="G19" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="H19" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="I19" s="56" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="38.25">
-      <c r="B20" s="56"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56">
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53">
         <v>2</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="G20" s="52" t="s">
-        <v>152</v>
-      </c>
-      <c r="H20" s="52" t="s">
-        <v>153</v>
-      </c>
-      <c r="I20" s="60" t="s">
-        <v>154</v>
+        <v>155</v>
+      </c>
+      <c r="G20" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="H20" s="49" t="s">
+        <v>157</v>
+      </c>
+      <c r="I20" s="57" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="62.25" customHeight="1">
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56">
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="53">
         <v>3</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="G21" s="52" t="s">
-        <v>157</v>
-      </c>
-      <c r="H21" s="52" t="s">
-        <v>158</v>
-      </c>
-      <c r="I21" s="61" t="s">
-        <v>159</v>
+        <v>160</v>
+      </c>
+      <c r="G21" s="49" t="s">
+        <v>161</v>
+      </c>
+      <c r="H21" s="49" t="s">
+        <v>162</v>
+      </c>
+      <c r="I21" s="58" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="37.5" customHeight="1">
-      <c r="B22" s="56"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56">
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="53">
         <v>4</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="G22" s="59" t="s">
-        <v>162</v>
-      </c>
-      <c r="H22" s="52" t="s">
-        <v>163</v>
-      </c>
-      <c r="I22" s="60" t="s">
-        <v>164</v>
+        <v>165</v>
+      </c>
+      <c r="G22" s="56" t="s">
+        <v>166</v>
+      </c>
+      <c r="H22" s="49" t="s">
+        <v>167</v>
+      </c>
+      <c r="I22" s="57" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="38.25" customHeight="1">
-      <c r="B23" s="56"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56">
+      <c r="B23" s="53"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53">
         <v>5</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="G23" s="53" t="s">
-        <v>167</v>
-      </c>
-      <c r="H23" s="53" t="s">
-        <v>168</v>
-      </c>
-      <c r="I23" s="62" t="s">
-        <v>169</v>
+        <v>170</v>
+      </c>
+      <c r="G23" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="H23" s="50" t="s">
+        <v>172</v>
+      </c>
+      <c r="I23" s="59" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="25.5">
-      <c r="B24" s="56"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56">
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53">
         <v>6</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="G24" s="53" t="s">
-        <v>172</v>
-      </c>
-      <c r="H24" s="52" t="s">
-        <v>173</v>
-      </c>
-      <c r="I24" s="59" t="s">
-        <v>174</v>
+        <v>175</v>
+      </c>
+      <c r="G24" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="H24" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="I24" s="56" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="32.25" customHeight="1">
-      <c r="B25" s="69"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56">
+      <c r="B25" s="66"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="53">
         <v>7</v>
       </c>
-      <c r="E25" s="63" t="s">
-        <v>175</v>
-      </c>
-      <c r="F25" s="63" t="s">
-        <v>176</v>
-      </c>
-      <c r="G25" s="53" t="s">
-        <v>177</v>
-      </c>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
+      <c r="E25" s="60" t="s">
+        <v>179</v>
+      </c>
+      <c r="F25" s="60" t="s">
+        <v>180</v>
+      </c>
+      <c r="G25" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="H25" s="50"/>
+      <c r="I25" s="50"/>
     </row>
     <row r="26" spans="2:9" ht="37.5" customHeight="1">
-      <c r="B26" s="56"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56">
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53">
         <v>8</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="G26" s="53" t="s">
-        <v>180</v>
-      </c>
-      <c r="H26" s="53" t="s">
-        <v>181</v>
-      </c>
-      <c r="I26" s="53" t="s">
-        <v>182</v>
+        <v>183</v>
+      </c>
+      <c r="G26" s="50" t="s">
+        <v>184</v>
+      </c>
+      <c r="H26" s="50" t="s">
+        <v>185</v>
+      </c>
+      <c r="I26" s="50" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="42" customHeight="1">
-      <c r="B27" s="56"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56">
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53">
         <v>9</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="G27" s="53" t="s">
-        <v>185</v>
-      </c>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53" t="s">
-        <v>186</v>
+        <v>188</v>
+      </c>
+      <c r="G27" s="50" t="s">
+        <v>189</v>
+      </c>
+      <c r="H27" s="50"/>
+      <c r="I27" s="50" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="38.25" customHeight="1">
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56">
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="53">
         <v>10</v>
       </c>
-      <c r="E28" s="57" t="s">
-        <v>187</v>
-      </c>
-      <c r="F28" s="57" t="s">
-        <v>188</v>
-      </c>
-      <c r="G28" s="57" t="s">
-        <v>189</v>
-      </c>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
+      <c r="E28" s="54" t="s">
+        <v>191</v>
+      </c>
+      <c r="F28" s="54" t="s">
+        <v>192</v>
+      </c>
+      <c r="G28" s="54" t="s">
+        <v>193</v>
+      </c>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
     </row>
     <row r="29" spans="2:9">
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="53"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="53"/>
-      <c r="I29" s="53"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
     </row>
     <row r="30" spans="2:9" ht="51">
-      <c r="B30" s="56">
+      <c r="B30" s="53">
         <v>2</v>
       </c>
-      <c r="C30" s="56" t="s">
-        <v>190</v>
-      </c>
-      <c r="D30" s="56">
+      <c r="C30" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="D30" s="53">
         <v>1</v>
       </c>
-      <c r="E30" s="57" t="s">
-        <v>191</v>
-      </c>
-      <c r="F30" s="57" t="s">
-        <v>146</v>
-      </c>
-      <c r="G30" s="58" t="s">
-        <v>147</v>
-      </c>
-      <c r="H30" s="58" t="s">
-        <v>148</v>
-      </c>
-      <c r="I30" s="59" t="s">
-        <v>149</v>
+      <c r="E30" s="54" t="s">
+        <v>195</v>
+      </c>
+      <c r="F30" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="G30" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="H30" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="I30" s="56" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="51">
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56">
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="53">
         <v>2</v>
       </c>
-      <c r="E31" s="53" t="s">
-        <v>192</v>
-      </c>
-      <c r="F31" s="53" t="s">
-        <v>193</v>
-      </c>
-      <c r="G31" s="52" t="s">
-        <v>194</v>
-      </c>
-      <c r="H31" s="52" t="s">
-        <v>195</v>
-      </c>
-      <c r="I31" s="53"/>
+      <c r="E31" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="F31" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="G31" s="49" t="s">
+        <v>198</v>
+      </c>
+      <c r="H31" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="I31" s="50"/>
     </row>
     <row r="32" spans="2:9" ht="51">
-      <c r="B32" s="56"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="56">
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53">
         <v>3</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="G32" s="53" t="s">
-        <v>198</v>
-      </c>
-      <c r="H32" s="52" t="s">
-        <v>199</v>
-      </c>
-      <c r="I32" s="52" t="s">
-        <v>200</v>
+        <v>201</v>
+      </c>
+      <c r="G32" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="H32" s="49" t="s">
+        <v>203</v>
+      </c>
+      <c r="I32" s="49" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="31.5" customHeight="1">
-      <c r="B33" s="56"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="56">
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53">
         <v>4</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="G33" s="53" t="s">
-        <v>203</v>
-      </c>
-      <c r="H33" s="52" t="s">
-        <v>204</v>
-      </c>
-      <c r="I33" s="52" t="s">
-        <v>205</v>
+        <v>206</v>
+      </c>
+      <c r="G33" s="50" t="s">
+        <v>207</v>
+      </c>
+      <c r="H33" s="49" t="s">
+        <v>208</v>
+      </c>
+      <c r="I33" s="49" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="34.5" customHeight="1">
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56">
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53">
         <v>5</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="G34" s="53" t="s">
-        <v>208</v>
-      </c>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53" t="s">
-        <v>209</v>
+        <v>211</v>
+      </c>
+      <c r="G34" s="50" t="s">
+        <v>212</v>
+      </c>
+      <c r="H34" s="50"/>
+      <c r="I34" s="50" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="48" customHeight="1">
-      <c r="B35" s="56"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56">
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53">
         <v>7</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="G35" s="53" t="s">
-        <v>172</v>
-      </c>
-      <c r="H35" s="52" t="s">
-        <v>173</v>
-      </c>
-      <c r="I35" s="62" t="s">
-        <v>212</v>
+        <v>215</v>
+      </c>
+      <c r="G35" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="H35" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="I35" s="59" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="39" customHeight="1">
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56">
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53">
         <v>8</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="G36" s="53" t="s">
-        <v>215</v>
-      </c>
-      <c r="H36" s="53" t="s">
-        <v>216</v>
-      </c>
-      <c r="I36" s="53" t="s">
-        <v>217</v>
+        <v>218</v>
+      </c>
+      <c r="G36" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="H36" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="I36" s="50" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="2:9" ht="37.5" customHeight="1">
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56">
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53">
         <v>9</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="G37" s="53" t="s">
-        <v>220</v>
-      </c>
-      <c r="H37" s="53" t="s">
-        <v>221</v>
-      </c>
-      <c r="I37" s="53" t="s">
-        <v>222</v>
+        <v>223</v>
+      </c>
+      <c r="G37" s="50" t="s">
+        <v>224</v>
+      </c>
+      <c r="H37" s="50" t="s">
+        <v>225</v>
+      </c>
+      <c r="I37" s="50" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="38" spans="2:9" ht="36.75" customHeight="1">
-      <c r="B38" s="56"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56">
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53">
         <v>10</v>
       </c>
-      <c r="E38" s="57" t="s">
-        <v>223</v>
-      </c>
-      <c r="F38" s="57" t="s">
-        <v>224</v>
-      </c>
-      <c r="G38" s="68" t="s">
-        <v>189</v>
-      </c>
-      <c r="H38" s="57"/>
-      <c r="I38" s="57"/>
+      <c r="E38" s="54" t="s">
+        <v>227</v>
+      </c>
+      <c r="F38" s="54" t="s">
+        <v>228</v>
+      </c>
+      <c r="G38" s="65" t="s">
+        <v>193</v>
+      </c>
+      <c r="H38" s="54"/>
+      <c r="I38" s="54"/>
     </row>
     <row r="39" spans="2:9" ht="12.75" customHeight="1">
-      <c r="B39" s="56"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="56"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
       <c r="E39" s="15"/>
       <c r="F39" s="15"/>
-      <c r="G39" s="62"/>
-      <c r="H39" s="53"/>
-      <c r="I39" s="53"/>
+      <c r="G39" s="59"/>
+      <c r="H39" s="50"/>
+      <c r="I39" s="50"/>
     </row>
     <row r="40" spans="2:9" ht="38.25">
-      <c r="B40" s="56">
+      <c r="B40" s="53">
         <v>3</v>
       </c>
-      <c r="C40" s="56" t="s">
-        <v>225</v>
-      </c>
-      <c r="D40" s="56">
+      <c r="C40" s="53" t="s">
+        <v>229</v>
+      </c>
+      <c r="D40" s="53">
         <v>1</v>
       </c>
-      <c r="E40" s="57" t="s">
-        <v>226</v>
-      </c>
-      <c r="F40" s="57" t="s">
-        <v>146</v>
-      </c>
-      <c r="G40" s="58" t="s">
-        <v>227</v>
-      </c>
-      <c r="H40" s="58" t="s">
-        <v>148</v>
-      </c>
-      <c r="I40" s="68" t="s">
-        <v>149</v>
+      <c r="E40" s="54" t="s">
+        <v>230</v>
+      </c>
+      <c r="F40" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="G40" s="55" t="s">
+        <v>231</v>
+      </c>
+      <c r="H40" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="I40" s="65" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="2:9" ht="27" customHeight="1">
-      <c r="B41" s="64"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="56">
+      <c r="B41" s="61"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53">
         <v>2</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="G41" s="52" t="s">
-        <v>230</v>
-      </c>
-      <c r="H41" s="52"/>
-      <c r="I41" s="53" t="s">
-        <v>231</v>
+        <v>233</v>
+      </c>
+      <c r="G41" s="49" t="s">
+        <v>234</v>
+      </c>
+      <c r="H41" s="49"/>
+      <c r="I41" s="50" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="42" spans="2:9" ht="30" customHeight="1">
-      <c r="B42" s="56"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="56">
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53">
         <v>3</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="G42" s="53" t="s">
-        <v>234</v>
-      </c>
-      <c r="H42" s="53" t="s">
-        <v>235</v>
-      </c>
-      <c r="I42" s="53" t="s">
-        <v>236</v>
+        <v>237</v>
+      </c>
+      <c r="G42" s="50" t="s">
+        <v>238</v>
+      </c>
+      <c r="H42" s="50" t="s">
+        <v>239</v>
+      </c>
+      <c r="I42" s="50" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="2:9" ht="30.75" customHeight="1">
-      <c r="B43" s="56"/>
-      <c r="C43" s="56"/>
-      <c r="D43" s="56">
+      <c r="B43" s="53"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53">
         <v>4</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="G43" s="53" t="s">
-        <v>239</v>
-      </c>
-      <c r="H43" s="53" t="s">
-        <v>240</v>
-      </c>
-      <c r="I43" s="53" t="s">
-        <v>241</v>
+        <v>242</v>
+      </c>
+      <c r="G43" s="50" t="s">
+        <v>243</v>
+      </c>
+      <c r="H43" s="50" t="s">
+        <v>244</v>
+      </c>
+      <c r="I43" s="50" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="44" spans="2:9" ht="36.75" customHeight="1">
-      <c r="B44" s="56"/>
-      <c r="C44" s="56"/>
-      <c r="D44" s="56">
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53">
         <v>5</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="G44" s="53" t="s">
-        <v>244</v>
-      </c>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53" t="s">
-        <v>245</v>
+        <v>247</v>
+      </c>
+      <c r="G44" s="50" t="s">
+        <v>248</v>
+      </c>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="45" spans="2:9" ht="39.75" customHeight="1">
-      <c r="B45" s="56"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="56">
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53">
         <v>6</v>
       </c>
-      <c r="E45" s="57" t="s">
-        <v>246</v>
-      </c>
-      <c r="F45" s="57" t="s">
-        <v>224</v>
-      </c>
-      <c r="G45" s="59" t="s">
-        <v>189</v>
-      </c>
-      <c r="H45" s="57"/>
-      <c r="I45" s="53"/>
+      <c r="E45" s="54" t="s">
+        <v>250</v>
+      </c>
+      <c r="F45" s="54" t="s">
+        <v>228</v>
+      </c>
+      <c r="G45" s="56" t="s">
+        <v>193</v>
+      </c>
+      <c r="H45" s="54"/>
+      <c r="I45" s="50"/>
     </row>
     <row r="46" spans="2:9" ht="15">
-      <c r="B46" s="56"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="65"/>
+      <c r="B46" s="53"/>
+      <c r="C46" s="53"/>
+      <c r="D46" s="53"/>
+      <c r="E46" s="62"/>
       <c r="F46" s="15"/>
-      <c r="G46" s="59"/>
-      <c r="H46" s="53"/>
-      <c r="I46" s="53"/>
+      <c r="G46" s="56"/>
+      <c r="H46" s="50"/>
+      <c r="I46" s="50"/>
     </row>
     <row r="47" spans="2:9" ht="38.25">
-      <c r="B47" s="56">
+      <c r="B47" s="53">
         <v>4</v>
       </c>
-      <c r="C47" s="56" t="s">
-        <v>247</v>
-      </c>
-      <c r="D47" s="56">
+      <c r="C47" s="53" t="s">
+        <v>251</v>
+      </c>
+      <c r="D47" s="53">
         <v>1</v>
       </c>
-      <c r="E47" s="66" t="s">
-        <v>248</v>
-      </c>
-      <c r="F47" s="66" t="s">
-        <v>146</v>
-      </c>
-      <c r="G47" s="58" t="s">
-        <v>227</v>
-      </c>
-      <c r="H47" s="58" t="s">
-        <v>148</v>
-      </c>
-      <c r="I47" s="59" t="s">
-        <v>149</v>
+      <c r="E47" s="63" t="s">
+        <v>252</v>
+      </c>
+      <c r="F47" s="63" t="s">
+        <v>150</v>
+      </c>
+      <c r="G47" s="55" t="s">
+        <v>231</v>
+      </c>
+      <c r="H47" s="55" t="s">
+        <v>152</v>
+      </c>
+      <c r="I47" s="56" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="48" spans="2:9" ht="30.75" customHeight="1">
-      <c r="B48" s="56"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="56">
+      <c r="B48" s="53"/>
+      <c r="C48" s="53"/>
+      <c r="D48" s="53">
         <v>2</v>
       </c>
-      <c r="E48" s="59" t="s">
-        <v>249</v>
-      </c>
-      <c r="F48" s="59" t="s">
-        <v>250</v>
-      </c>
-      <c r="G48" s="52" t="s">
-        <v>251</v>
-      </c>
-      <c r="H48" s="67" t="s">
-        <v>252</v>
-      </c>
-      <c r="I48" s="52" t="s">
+      <c r="E48" s="56" t="s">
         <v>253</v>
+      </c>
+      <c r="F48" s="56" t="s">
+        <v>254</v>
+      </c>
+      <c r="G48" s="49" t="s">
+        <v>255</v>
+      </c>
+      <c r="H48" s="64" t="s">
+        <v>256</v>
+      </c>
+      <c r="I48" s="49" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="2:9" ht="29.25" customHeight="1">
-      <c r="B49" s="56"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="56">
+      <c r="B49" s="53"/>
+      <c r="C49" s="53"/>
+      <c r="D49" s="53">
         <v>3</v>
       </c>
-      <c r="E49" s="59" t="s">
-        <v>254</v>
+      <c r="E49" s="56" t="s">
+        <v>258</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>255</v>
-      </c>
-      <c r="G49" s="53" t="s">
-        <v>256</v>
-      </c>
-      <c r="H49" s="55" t="s">
-        <v>257</v>
-      </c>
-      <c r="I49" s="53" t="s">
-        <v>258</v>
+        <v>259</v>
+      </c>
+      <c r="G49" s="50" t="s">
+        <v>260</v>
+      </c>
+      <c r="H49" s="52" t="s">
+        <v>261</v>
+      </c>
+      <c r="I49" s="50" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="50" spans="2:9" ht="28.5" customHeight="1">
-      <c r="B50" s="56"/>
-      <c r="C50" s="56"/>
-      <c r="D50" s="56">
+      <c r="B50" s="53"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53">
         <v>4</v>
       </c>
-      <c r="E50" s="59" t="s">
-        <v>259</v>
+      <c r="E50" s="56" t="s">
+        <v>263</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="G50" s="53" t="s">
-        <v>261</v>
-      </c>
-      <c r="H50" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="I50" s="53" t="s">
-        <v>263</v>
+        <v>264</v>
+      </c>
+      <c r="G50" s="50" t="s">
+        <v>265</v>
+      </c>
+      <c r="H50" s="50" t="s">
+        <v>266</v>
+      </c>
+      <c r="I50" s="50" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="51" spans="2:9" ht="32.25" customHeight="1">
-      <c r="B51" s="56"/>
-      <c r="C51" s="56"/>
-      <c r="D51" s="56">
+      <c r="B51" s="53"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="53">
         <v>5</v>
       </c>
-      <c r="E51" s="57" t="s">
-        <v>264</v>
-      </c>
-      <c r="F51" s="57" t="s">
-        <v>224</v>
-      </c>
-      <c r="G51" s="59" t="s">
-        <v>189</v>
-      </c>
-      <c r="H51" s="57"/>
-      <c r="I51" s="57"/>
+      <c r="E51" s="54" t="s">
+        <v>268</v>
+      </c>
+      <c r="F51" s="54" t="s">
+        <v>228</v>
+      </c>
+      <c r="G51" s="56" t="s">
+        <v>193</v>
+      </c>
+      <c r="H51" s="54"/>
+      <c r="I51" s="54"/>
     </row>
     <row r="52" spans="2:9">
-      <c r="B52" s="56"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="56"/>
+      <c r="B52" s="53"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="53"/>
       <c r="E52" s="15"/>
       <c r="F52" s="15"/>
-      <c r="G52" s="59"/>
-      <c r="H52" s="53"/>
-      <c r="I52" s="53"/>
+      <c r="G52" s="56"/>
+      <c r="H52" s="50"/>
+      <c r="I52" s="50"/>
     </row>
     <row r="54" spans="2:9">
-      <c r="H54" s="54"/>
+      <c r="H54" s="51"/>
     </row>
     <row r="55" spans="2:9">
-      <c r="H55" s="54"/>
+      <c r="H55" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -37098,50 +37261,50 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="15">
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
     </row>
     <row r="3" spans="1:10" ht="15">
-      <c r="B3" s="75" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
+      <c r="B3" s="91" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
     </row>
     <row r="4" spans="1:10">
       <c r="B4" s="27" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C4" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="D4" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="G4" t="s">
         <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="I4" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="J4" s="28" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -37156,22 +37319,22 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="F5" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="G5" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H5">
         <v>9876781234</v>
       </c>
       <c r="I5" s="29" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="J5" s="28" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -37186,22 +37349,22 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="F6" t="s">
+        <v>282</v>
+      </c>
+      <c r="G6" t="s">
         <v>278</v>
-      </c>
-      <c r="G6" t="s">
-        <v>274</v>
       </c>
       <c r="H6">
         <v>9129867850</v>
       </c>
       <c r="I6" s="29" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="J6" s="28" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -37221,43 +37384,43 @@
       <c r="F9" s="33"/>
     </row>
     <row r="11" spans="1:10" ht="15">
-      <c r="B11" s="71" t="s">
-        <v>281</v>
-      </c>
-      <c r="C11" s="76" t="s">
-        <v>282</v>
-      </c>
-      <c r="D11" s="76"/>
-      <c r="F11" s="77" t="s">
-        <v>283</v>
-      </c>
-      <c r="G11" s="77"/>
-      <c r="I11" s="77" t="s">
-        <v>284</v>
-      </c>
-      <c r="J11" s="77"/>
+      <c r="B11" s="68" t="s">
+        <v>285</v>
+      </c>
+      <c r="C11" s="92" t="s">
+        <v>286</v>
+      </c>
+      <c r="D11" s="92"/>
+      <c r="F11" s="93" t="s">
+        <v>287</v>
+      </c>
+      <c r="G11" s="93"/>
+      <c r="I11" s="93" t="s">
+        <v>288</v>
+      </c>
+      <c r="J11" s="93"/>
     </row>
     <row r="12" spans="1:10">
       <c r="B12" s="34" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="I12" s="36" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="J12" s="37" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15">
@@ -37268,20 +37431,20 @@
         <v>1</v>
       </c>
       <c r="D13" s="28" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="E13" s="33"/>
       <c r="F13" s="38">
         <v>1</v>
       </c>
       <c r="G13" s="39" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="I13" s="38">
         <v>3</v>
       </c>
       <c r="J13" s="39" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -37292,19 +37455,19 @@
         <v>2</v>
       </c>
       <c r="D14" s="28" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="F14" s="38">
         <v>2</v>
       </c>
       <c r="G14" s="39" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="I14" s="38">
         <v>4</v>
       </c>
       <c r="J14" s="39" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -37317,7 +37480,7 @@
         <v>5</v>
       </c>
       <c r="J15" s="41" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="15">
@@ -37329,25 +37492,25 @@
       <c r="B21" s="33"/>
     </row>
     <row r="22" spans="2:9" ht="15">
-      <c r="B22" s="75" t="s">
-        <v>297</v>
-      </c>
-      <c r="C22" s="78"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="79"/>
+      <c r="B22" s="91" t="s">
+        <v>301</v>
+      </c>
+      <c r="C22" s="94"/>
+      <c r="D22" s="94"/>
+      <c r="E22" s="95"/>
     </row>
     <row r="23" spans="2:9">
       <c r="B23" s="38" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="C23" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="D23" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="E23" s="39" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="24" spans="2:9">
@@ -37358,7 +37521,7 @@
         <v>36962</v>
       </c>
       <c r="D24" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="E24" s="44">
         <v>44177</v>
@@ -37372,7 +37535,7 @@
         <v>36770</v>
       </c>
       <c r="D25" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="E25" s="44">
         <v>43580</v>
@@ -37386,39 +37549,39 @@
       <c r="E26" s="41"/>
     </row>
     <row r="28" spans="2:9" ht="15">
-      <c r="B28" s="80" t="s">
-        <v>303</v>
-      </c>
-      <c r="C28" s="80"/>
-      <c r="D28" s="80"/>
-      <c r="E28" s="80"/>
+      <c r="B28" s="96" t="s">
+        <v>307</v>
+      </c>
+      <c r="C28" s="96"/>
+      <c r="D28" s="96"/>
+      <c r="E28" s="96"/>
       <c r="F28" s="35"/>
-      <c r="H28" s="81" t="s">
-        <v>304</v>
-      </c>
-      <c r="I28" s="82"/>
+      <c r="H28" s="97" t="s">
+        <v>308</v>
+      </c>
+      <c r="I28" s="98"/>
     </row>
     <row r="29" spans="2:9">
       <c r="B29" s="34" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="D29" s="46" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="E29" s="46" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="H29" s="38" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="I29" s="39" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row r="30" spans="2:9">
@@ -37441,7 +37604,7 @@
         <v>1</v>
       </c>
       <c r="I30" s="39" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="31" spans="2:9">
@@ -37464,7 +37627,7 @@
         <v>2</v>
       </c>
       <c r="I31" s="39" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
     </row>
     <row r="32" spans="2:9">
@@ -37487,41 +37650,41 @@
         <v>3</v>
       </c>
       <c r="I32" s="41" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15">
       <c r="B35" s="34"/>
-      <c r="C35" s="73"/>
-      <c r="F35" s="76" t="s">
-        <v>314</v>
-      </c>
-      <c r="G35" s="83"/>
-      <c r="H35" s="83"/>
-      <c r="I35" s="83"/>
-      <c r="J35" s="84"/>
+      <c r="C35" s="70"/>
+      <c r="F35" s="92" t="s">
+        <v>318</v>
+      </c>
+      <c r="G35" s="99"/>
+      <c r="H35" s="99"/>
+      <c r="I35" s="99"/>
+      <c r="J35" s="100"/>
     </row>
     <row r="36" spans="2:10">
       <c r="B36" s="34" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="F36" s="36" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="G36" s="42" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="H36" s="42" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="I36" s="42" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="J36" s="37" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="37" spans="2:10">
@@ -37535,10 +37698,10 @@
         <v>1</v>
       </c>
       <c r="G37" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="H37" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="I37">
         <v>2019</v>
@@ -37558,10 +37721,10 @@
         <v>2</v>
       </c>
       <c r="G38" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="H38" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="I38">
         <v>2020</v>
@@ -37588,48 +37751,48 @@
       <c r="C40" s="32"/>
     </row>
     <row r="41" spans="2:10" ht="15">
-      <c r="F41" s="76" t="s">
-        <v>324</v>
-      </c>
-      <c r="G41" s="83"/>
-      <c r="H41" s="84"/>
+      <c r="F41" s="92" t="s">
+        <v>328</v>
+      </c>
+      <c r="G41" s="99"/>
+      <c r="H41" s="100"/>
     </row>
     <row r="42" spans="2:10">
       <c r="F42" s="36" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="G42" s="42" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="H42" s="37" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="15">
-      <c r="B43" s="80" t="s">
-        <v>328</v>
-      </c>
-      <c r="C43" s="86"/>
+      <c r="B43" s="96" t="s">
+        <v>332</v>
+      </c>
+      <c r="C43" s="102"/>
       <c r="F43" s="38">
         <v>1</v>
       </c>
       <c r="G43" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="H43" s="39"/>
     </row>
     <row r="44" spans="2:10">
       <c r="B44" s="34" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="C44" s="35" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="F44" s="38">
         <v>2</v>
       </c>
       <c r="G44" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="H44" s="39"/>
     </row>
@@ -37644,7 +37807,7 @@
         <v>3</v>
       </c>
       <c r="G45" s="45" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="H45" s="41"/>
     </row>
@@ -37665,77 +37828,77 @@
       </c>
     </row>
     <row r="50" spans="2:22" ht="15">
-      <c r="B50" s="76" t="s">
-        <v>334</v>
-      </c>
-      <c r="C50" s="83"/>
-      <c r="D50" s="83"/>
-      <c r="E50" s="83"/>
+      <c r="B50" s="92" t="s">
+        <v>338</v>
+      </c>
+      <c r="C50" s="99"/>
+      <c r="D50" s="99"/>
+      <c r="E50" s="99"/>
       <c r="F50" s="37"/>
-      <c r="H50" s="76" t="s">
-        <v>335</v>
-      </c>
-      <c r="I50" s="84"/>
+      <c r="H50" s="92" t="s">
+        <v>339</v>
+      </c>
+      <c r="I50" s="100"/>
       <c r="K50" s="36"/>
-      <c r="L50" s="83" t="s">
-        <v>336</v>
-      </c>
-      <c r="M50" s="84"/>
-      <c r="O50" s="76" t="s">
+      <c r="L50" s="99" t="s">
+        <v>340</v>
+      </c>
+      <c r="M50" s="100"/>
+      <c r="O50" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="P50" s="84"/>
-      <c r="R50" s="80" t="s">
-        <v>337</v>
-      </c>
-      <c r="S50" s="85"/>
-      <c r="T50" s="86"/>
+      <c r="P50" s="100"/>
+      <c r="R50" s="96" t="s">
+        <v>341</v>
+      </c>
+      <c r="S50" s="101"/>
+      <c r="T50" s="102"/>
       <c r="U50" s="33"/>
       <c r="V50" s="33"/>
     </row>
     <row r="51" spans="2:22">
       <c r="B51" s="36" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="C51" s="42" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="D51" s="42" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="E51" s="42" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="F51" s="37" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="H51" s="36" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="I51" s="37" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="K51" s="38"/>
       <c r="L51" t="s">
+        <v>348</v>
+      </c>
+      <c r="M51" s="39" t="s">
+        <v>349</v>
+      </c>
+      <c r="O51" s="38" t="s">
+        <v>345</v>
+      </c>
+      <c r="P51" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="R51" s="34" t="s">
         <v>344</v>
       </c>
-      <c r="M51" s="39" t="s">
-        <v>345</v>
-      </c>
-      <c r="O51" s="38" t="s">
-        <v>341</v>
-      </c>
-      <c r="P51" s="39" t="s">
-        <v>346</v>
-      </c>
-      <c r="R51" s="34" t="s">
-        <v>340</v>
-      </c>
       <c r="S51" s="46" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="T51" s="35" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="52" spans="2:22">
@@ -37758,20 +37921,20 @@
         <v>500</v>
       </c>
       <c r="I52" s="39" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="K52" s="38"/>
       <c r="L52">
         <v>600</v>
       </c>
       <c r="M52" s="39" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="O52" s="38">
         <v>200</v>
       </c>
       <c r="P52" s="39" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="R52" s="27">
         <v>1</v>
@@ -37803,20 +37966,20 @@
         <v>501</v>
       </c>
       <c r="I53" s="39" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="K53" s="38"/>
       <c r="L53">
         <v>601</v>
       </c>
       <c r="M53" s="39" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="O53" s="38">
         <v>201</v>
       </c>
       <c r="P53" s="39" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="R53" s="27">
         <v>2</v>
@@ -37848,20 +38011,20 @@
         <v>502</v>
       </c>
       <c r="I54" s="39" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="K54" s="38"/>
       <c r="L54">
         <v>602</v>
       </c>
       <c r="M54" s="39" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="O54" s="38">
         <v>202</v>
       </c>
       <c r="P54" s="39" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="R54" s="27"/>
       <c r="T54" s="28"/>
@@ -37879,60 +38042,60 @@
         <v>603</v>
       </c>
       <c r="M55" s="41" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="O55" s="40">
         <v>203</v>
       </c>
       <c r="P55" s="41" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="R55" s="30"/>
       <c r="S55" s="31"/>
       <c r="T55" s="32"/>
     </row>
     <row r="62" spans="2:22" ht="15">
-      <c r="B62" s="81" t="s">
-        <v>358</v>
-      </c>
-      <c r="C62" s="87"/>
-      <c r="D62" s="87"/>
+      <c r="B62" s="97" t="s">
+        <v>362</v>
+      </c>
+      <c r="C62" s="103"/>
+      <c r="D62" s="103"/>
       <c r="E62" s="48"/>
-      <c r="H62" s="80" t="s">
-        <v>359</v>
-      </c>
-      <c r="I62" s="85"/>
-      <c r="J62" s="85"/>
-      <c r="K62" s="85"/>
-      <c r="L62" s="86"/>
+      <c r="H62" s="96" t="s">
+        <v>363</v>
+      </c>
+      <c r="I62" s="101"/>
+      <c r="J62" s="101"/>
+      <c r="K62" s="101"/>
+      <c r="L62" s="102"/>
     </row>
     <row r="63" spans="2:22">
       <c r="B63" s="27" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="C63" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="D63" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="E63" s="28" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="H63" s="34" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="I63" s="46" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="J63" s="46" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="K63" s="46" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="L63" s="35" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="64" spans="2:22">
@@ -37940,7 +38103,7 @@
         <v>1</v>
       </c>
       <c r="C64" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="D64">
         <v>1</v>
@@ -37952,10 +38115,10 @@
         <v>1</v>
       </c>
       <c r="I64" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="J64" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="K64">
         <v>2019</v>
@@ -37969,7 +38132,7 @@
         <v>2</v>
       </c>
       <c r="C65" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="D65">
         <v>2</v>
@@ -37981,10 +38144,10 @@
         <v>2</v>
       </c>
       <c r="I65" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="J65" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="K65">
         <v>2020</v>
@@ -37998,7 +38161,7 @@
         <v>3</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="D66" s="31">
         <v>1</v>
@@ -38013,35 +38176,35 @@
       <c r="L66" s="32"/>
     </row>
     <row r="68" spans="2:12" ht="15">
-      <c r="F68" s="76" t="s">
-        <v>368</v>
-      </c>
-      <c r="G68" s="84"/>
+      <c r="F68" s="92" t="s">
+        <v>372</v>
+      </c>
+      <c r="G68" s="100"/>
     </row>
     <row r="69" spans="2:12" ht="15">
-      <c r="B69" s="80" t="s">
-        <v>369</v>
-      </c>
-      <c r="C69" s="86"/>
+      <c r="B69" s="96" t="s">
+        <v>373</v>
+      </c>
+      <c r="C69" s="102"/>
       <c r="F69" s="36" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="G69" s="37" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
     </row>
     <row r="70" spans="2:12">
       <c r="B70" s="34" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="C70" s="35" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="F70" s="38">
         <v>278</v>
       </c>
       <c r="G70" s="39" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row r="71" spans="2:12">
@@ -38055,7 +38218,7 @@
         <v>279</v>
       </c>
       <c r="G71" s="39" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
     </row>
     <row r="72" spans="2:12">
@@ -38069,7 +38232,7 @@
         <v>280</v>
       </c>
       <c r="G72" s="39" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row r="73" spans="2:12">
@@ -38083,18 +38246,18 @@
       <c r="G73" s="41"/>
     </row>
     <row r="76" spans="2:12" ht="15">
-      <c r="B76" s="70"/>
-      <c r="F76" s="80" t="s">
-        <v>377</v>
-      </c>
-      <c r="G76" s="86"/>
+      <c r="B76" s="67"/>
+      <c r="F76" s="96" t="s">
+        <v>381</v>
+      </c>
+      <c r="G76" s="102"/>
     </row>
     <row r="77" spans="2:12">
       <c r="F77" s="34" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="G77" s="35" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="78" spans="2:12">
@@ -38102,7 +38265,7 @@
         <v>1</v>
       </c>
       <c r="G78" s="28" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row r="79" spans="2:12">
@@ -38110,7 +38273,7 @@
         <v>2</v>
       </c>
       <c r="G79" s="28" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
     </row>
     <row r="80" spans="2:12">
@@ -38122,37 +38285,37 @@
       <c r="G81" s="32"/>
     </row>
     <row r="87" spans="2:9" ht="15">
-      <c r="B87" s="76" t="s">
-        <v>382</v>
-      </c>
-      <c r="C87" s="84"/>
-      <c r="E87" s="77" t="s">
+      <c r="B87" s="92" t="s">
+        <v>386</v>
+      </c>
+      <c r="C87" s="100"/>
+      <c r="E87" s="93" t="s">
         <v>15</v>
       </c>
-      <c r="F87" s="88"/>
-      <c r="H87" s="76" t="s">
+      <c r="F87" s="104"/>
+      <c r="H87" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="I87" s="84"/>
+      <c r="I87" s="100"/>
     </row>
     <row r="88" spans="2:9">
       <c r="B88" s="36" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="C88" s="37" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="E88" s="36" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="F88" s="37" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="H88" s="36" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="I88" s="37" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="89" spans="2:9">
@@ -38166,13 +38329,13 @@
         <v>1</v>
       </c>
       <c r="F89" s="39" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="H89" s="38">
         <v>10</v>
       </c>
       <c r="I89" s="39" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row r="90" spans="2:9">
@@ -38186,13 +38349,13 @@
         <v>2</v>
       </c>
       <c r="F90" s="39" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="H90" s="38">
         <v>11</v>
       </c>
       <c r="I90" s="39" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="91" spans="2:9">
@@ -38206,13 +38369,13 @@
         <v>3</v>
       </c>
       <c r="F91" s="39" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="H91" s="38">
         <v>12</v>
       </c>
       <c r="I91" s="39" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row r="92" spans="2:9">
@@ -38224,13 +38387,13 @@
       <c r="I92" s="41"/>
     </row>
     <row r="96" spans="2:9" ht="15">
-      <c r="B96" s="72" t="s">
-        <v>393</v>
+      <c r="B96" s="69" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="97" spans="2:2">
       <c r="B97" s="36" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="98" spans="2:2">
@@ -38252,13 +38415,13 @@
       <c r="B101" s="40"/>
     </row>
     <row r="105" spans="2:2" ht="15">
-      <c r="B105" s="71" t="s">
-        <v>395</v>
+      <c r="B105" s="68" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="106" spans="2:2">
       <c r="B106" s="27" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="107" spans="2:2">
@@ -38280,17 +38443,17 @@
       <c r="B110" s="30"/>
     </row>
     <row r="115" spans="2:3" ht="15">
-      <c r="B115" s="76" t="s">
-        <v>397</v>
-      </c>
-      <c r="C115" s="84"/>
+      <c r="B115" s="92" t="s">
+        <v>401</v>
+      </c>
+      <c r="C115" s="100"/>
     </row>
     <row r="116" spans="2:3">
       <c r="B116" s="34" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="C116" s="35" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row r="117" spans="2:3">
@@ -38355,15 +38518,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D3CFBF-880F-481E-9D27-6F5C85AAC27F}">
   <dimension ref="V29"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="AF18" sqref="AF18"/>
+    <sheetView topLeftCell="D216" workbookViewId="0">
+      <selection activeCell="L176" sqref="L176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="29" spans="22:22">
       <c r="V29" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -38384,28 +38547,28 @@
   <sheetData>
     <row r="1" spans="3:10" ht="23.25">
       <c r="J1" s="12" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="3:10" ht="20.25">
       <c r="C4" s="11" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D4" s="6"/>
     </row>
     <row r="6" spans="3:10" ht="20.25">
       <c r="D6" s="10" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
     </row>
     <row r="21" spans="4:4" ht="20.25">
       <c r="D21" s="10" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="33" spans="4:8" ht="20.25">
       <c r="D33" s="13" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
     </row>
     <row r="38" spans="4:8">
@@ -38413,34 +38576,34 @@
     </row>
     <row r="46" spans="4:8" ht="20.25">
       <c r="D46" s="10" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
     </row>
     <row r="59" spans="3:4" ht="20.25">
       <c r="C59" s="11" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D59" s="10"/>
     </row>
     <row r="61" spans="3:4" ht="20.25">
       <c r="D61" s="10" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
     </row>
     <row r="74" spans="4:5" ht="20.25">
       <c r="D74" s="10" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="E74" s="10"/>
     </row>
     <row r="85" spans="4:4" ht="20.25">
       <c r="D85" s="10" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row r="296" spans="3:5" ht="18">
       <c r="C296" s="9" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="D296" s="9"/>
       <c r="E296" s="9"/>
@@ -38472,7 +38635,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15">
       <c r="A1" s="22" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -38480,100 +38643,100 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B3" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="F3" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B5" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1">
       <c r="B6" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:6">
       <c r="B7" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="B9" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B10" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B12" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15">
       <c r="A16" s="22" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B17" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B19" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="B20" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B22" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B24" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15">
@@ -38599,106 +38762,106 @@
     </row>
     <row r="64" spans="1:1" ht="15">
       <c r="A64" s="22" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="6" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B68" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="B69" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="6" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B74" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B76" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="B77" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="6" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B82" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="B83" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="15">
       <c r="A85" s="22" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="B86" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="B88" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -38727,10 +38890,10 @@
     <row r="1" spans="1:3">
       <c r="A1" s="17"/>
       <c r="B1" s="18" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -38740,47 +38903,47 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="15" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="15"/>
       <c r="B4" s="16" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="15"/>
       <c r="B5" s="16" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="15"/>
       <c r="B6" s="16" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="15" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -38835,10 +38998,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="15" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>4</v>
@@ -38847,31 +39010,31 @@
     <row r="19" spans="1:4">
       <c r="A19" s="15"/>
       <c r="B19" s="16" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="15"/>
       <c r="B20" s="16" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="D20" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="15"/>
       <c r="B21" s="16" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -38893,7 +39056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC21BEB0-7817-4402-83E4-96DD5F41634F}">
   <dimension ref="A3:O79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -38905,128 +39068,128 @@
   <sheetData>
     <row r="3" spans="1:15" ht="20.25">
       <c r="L3" s="10" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="B9" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="O9" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="B11" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="B13" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B15" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="B17" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="O17" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B19" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="B21" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="B23" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="B25" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="O25" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
     </row>
     <row r="32" spans="1:15">
       <c r="O32" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
     </row>
     <row r="39" spans="15:15">
       <c r="O39" s="20" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
     </row>
     <row r="47" spans="15:15">
       <c r="O47" s="20" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="55" spans="15:15">
       <c r="O55" s="20" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
     </row>
     <row r="63" spans="15:15">
       <c r="O63" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
     </row>
     <row r="71" spans="15:15">
       <c r="O71" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
     </row>
     <row r="79" spans="15:15">
       <c r="O79" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated MOM _ Yoga
</commit_message>
<xml_diff>
--- a/Requirements/User story_Team genesis.xlsx
+++ b/Requirements/User story_Team genesis.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25216"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1D0BC73-26BA-4656-8AA3-647340CC12B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4FF02EB4-BC07-4B42-A6F1-2CF1257F7E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Modules" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="472">
   <si>
     <t>Modules and Attributes</t>
   </si>
@@ -500,6 +500,36 @@
   </si>
   <si>
     <t>Add profilers email in request to update</t>
+  </si>
+  <si>
+    <t>Estimation for UI implementation, Code reviews, testing</t>
+  </si>
+  <si>
+    <t>Remove list for awards and certificates</t>
+  </si>
+  <si>
+    <t>Define method for populating values when editing</t>
+  </si>
+  <si>
+    <t>Check whether the filters are and/or operations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In share and request to update, pass profile_id </t>
+  </si>
+  <si>
+    <t>Define method for getting recent profile in profile history</t>
+  </si>
+  <si>
+    <t>Estimation for page integration and code merging - 4 hours/2days</t>
+  </si>
+  <si>
+    <t>Compatability testing 3 hours</t>
+  </si>
+  <si>
+    <t>Swagger documentation 30-40 hours</t>
+  </si>
+  <si>
+    <t>WEB API Integration, Service Implementation, Service validation</t>
   </si>
   <si>
     <t>Team Genesis - Profile Management Project</t>
@@ -2230,6 +2260,15 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2237,15 +2276,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2260,10 +2290,16 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2282,12 +2318,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -35667,10 +35697,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C117"/>
+  <dimension ref="A1:C129"/>
   <sheetViews>
-    <sheetView topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A126" sqref="A126:C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -36460,6 +36490,80 @@
       <c r="B117" s="60"/>
       <c r="C117" s="61" t="s">
         <v>154</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A119" s="62">
+        <v>44617</v>
+      </c>
+      <c r="B119" s="63"/>
+      <c r="C119" s="64" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A120" s="56"/>
+      <c r="B120" s="23"/>
+      <c r="C120" s="58" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A121" s="56"/>
+      <c r="B121" s="23"/>
+      <c r="C121" s="58" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A122" s="56"/>
+      <c r="B122" s="23"/>
+      <c r="C122" s="58" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A123" s="56"/>
+      <c r="B123" s="23"/>
+      <c r="C123" s="58" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A124" s="59"/>
+      <c r="B124" s="60"/>
+      <c r="C124" s="61" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A126" s="62">
+        <v>44677</v>
+      </c>
+      <c r="B126" s="63"/>
+      <c r="C126" s="64" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A127" s="56"/>
+      <c r="B127" s="23"/>
+      <c r="C127" s="58" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A128" s="56"/>
+      <c r="B128" s="23"/>
+      <c r="C128" s="58" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A129" s="59"/>
+      <c r="B129" s="60"/>
+      <c r="C129" s="61" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -36489,7 +36593,7 @@
   <sheetData>
     <row r="5" spans="1:5">
       <c r="E5" s="8" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -36497,33 +36601,33 @@
     </row>
     <row r="10" spans="1:5">
       <c r="E10" s="8" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="2:9">
       <c r="B18" s="39" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="F18" s="39" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="51">
@@ -36531,25 +36635,25 @@
         <v>1</v>
       </c>
       <c r="C19" s="39" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="D19" s="39">
         <v>1</v>
       </c>
       <c r="E19" s="40" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="F19" s="40" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="G19" s="41" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="H19" s="41" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="I19" s="42" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="38.25">
@@ -36559,19 +36663,19 @@
         <v>2</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="G20" s="35" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="H20" s="35" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="I20" s="43" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="62.25" customHeight="1">
@@ -36581,19 +36685,19 @@
         <v>3</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="H21" s="35" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
       <c r="I21" s="44" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="37.5" customHeight="1">
@@ -36603,19 +36707,19 @@
         <v>4</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
       <c r="G22" s="42" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="H22" s="35" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="I22" s="43" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="38.25" customHeight="1">
@@ -36625,19 +36729,19 @@
         <v>5</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="G23" s="36" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="H23" s="36" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="I23" s="45" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="25.5">
@@ -36647,19 +36751,19 @@
         <v>6</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
       <c r="G24" s="36" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="H24" s="35" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="I24" s="42" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="32.25" customHeight="1">
@@ -36669,13 +36773,13 @@
         <v>7</v>
       </c>
       <c r="E25" s="46" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="F25" s="46" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="G25" s="36" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
       <c r="H25" s="36"/>
       <c r="I25" s="36"/>
@@ -36687,19 +36791,19 @@
         <v>8</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="G26" s="36" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="H26" s="36" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="I26" s="36" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="42" customHeight="1">
@@ -36709,17 +36813,17 @@
         <v>9</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="F27" s="15" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="G27" s="36" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="H27" s="36"/>
       <c r="I27" s="36" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
     <row r="28" spans="2:9" ht="38.25" customHeight="1">
@@ -36729,13 +36833,13 @@
         <v>10</v>
       </c>
       <c r="E28" s="40" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="F28" s="40" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="G28" s="40" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="H28" s="40"/>
       <c r="I28" s="40"/>
@@ -36755,25 +36859,25 @@
         <v>2</v>
       </c>
       <c r="C30" s="39" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="D30" s="39">
         <v>1</v>
       </c>
       <c r="E30" s="40" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="F30" s="40" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="G30" s="41" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="H30" s="41" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="I30" s="42" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="2:9" ht="51">
@@ -36783,16 +36887,16 @@
         <v>2</v>
       </c>
       <c r="E31" s="36" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
       <c r="F31" s="36" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="G31" s="35" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="H31" s="35" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="I31" s="36"/>
     </row>
@@ -36803,19 +36907,19 @@
         <v>3</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="G32" s="36" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="H32" s="35" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="I32" s="35" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="2:9" ht="31.5" customHeight="1">
@@ -36825,19 +36929,19 @@
         <v>4</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="G33" s="36" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="H33" s="35" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
       <c r="I33" s="35" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="34.5" customHeight="1">
@@ -36847,17 +36951,17 @@
         <v>5</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="G34" s="36" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="H34" s="36"/>
       <c r="I34" s="36" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="2:9" ht="48" customHeight="1">
@@ -36867,19 +36971,19 @@
         <v>7</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>232</v>
+        <v>242</v>
       </c>
       <c r="G35" s="36" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
       <c r="H35" s="35" t="s">
-        <v>194</v>
+        <v>204</v>
       </c>
       <c r="I35" s="45" t="s">
-        <v>233</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="2:9" ht="39" customHeight="1">
@@ -36889,19 +36993,19 @@
         <v>8</v>
       </c>
       <c r="E36" s="15" t="s">
-        <v>234</v>
+        <v>244</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>235</v>
+        <v>245</v>
       </c>
       <c r="G36" s="36" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="H36" s="36" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="I36" s="36" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
     </row>
     <row r="37" spans="2:9" ht="37.5" customHeight="1">
@@ -36911,19 +37015,19 @@
         <v>9</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="G37" s="36" t="s">
-        <v>241</v>
+        <v>251</v>
       </c>
       <c r="H37" s="36" t="s">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="I37" s="36" t="s">
-        <v>243</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="2:9" ht="36.75" customHeight="1">
@@ -36933,13 +37037,13 @@
         <v>10</v>
       </c>
       <c r="E38" s="40" t="s">
-        <v>244</v>
+        <v>254</v>
       </c>
       <c r="F38" s="40" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="G38" s="51" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="H38" s="40"/>
       <c r="I38" s="40"/>
@@ -36959,25 +37063,25 @@
         <v>3</v>
       </c>
       <c r="C40" s="39" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="D40" s="39">
         <v>1</v>
       </c>
       <c r="E40" s="40" t="s">
-        <v>247</v>
+        <v>257</v>
       </c>
       <c r="F40" s="40" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="G40" s="41" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="H40" s="41" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="I40" s="51" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="2:9" ht="27" customHeight="1">
@@ -36987,17 +37091,17 @@
         <v>2</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="G41" s="35" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="H41" s="35"/>
       <c r="I41" s="36" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
     </row>
     <row r="42" spans="2:9" ht="30" customHeight="1">
@@ -37007,19 +37111,19 @@
         <v>3</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="G42" s="36" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="H42" s="36" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="I42" s="36" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
     </row>
     <row r="43" spans="2:9" ht="30.75" customHeight="1">
@@ -37029,19 +37133,19 @@
         <v>4</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>258</v>
+        <v>268</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="G43" s="36" t="s">
-        <v>260</v>
+        <v>270</v>
       </c>
       <c r="H43" s="36" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="I43" s="36" t="s">
-        <v>262</v>
+        <v>272</v>
       </c>
     </row>
     <row r="44" spans="2:9" ht="36.75" customHeight="1">
@@ -37051,17 +37155,17 @@
         <v>5</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="G44" s="36" t="s">
-        <v>265</v>
+        <v>275</v>
       </c>
       <c r="H44" s="36"/>
       <c r="I44" s="36" t="s">
-        <v>266</v>
+        <v>276</v>
       </c>
     </row>
     <row r="45" spans="2:9" ht="39.75" customHeight="1">
@@ -37071,13 +37175,13 @@
         <v>6</v>
       </c>
       <c r="E45" s="40" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="F45" s="40" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="G45" s="42" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="H45" s="40"/>
       <c r="I45" s="36"/>
@@ -37097,25 +37201,25 @@
         <v>4</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
       <c r="D47" s="39">
         <v>1</v>
       </c>
       <c r="E47" s="49" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
       <c r="F47" s="49" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="G47" s="41" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="H47" s="41" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="I47" s="42" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48" spans="2:9" ht="30.75" customHeight="1">
@@ -37125,19 +37229,19 @@
         <v>2</v>
       </c>
       <c r="E48" s="42" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
       <c r="F48" s="42" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
       <c r="G48" s="35" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
       <c r="H48" s="50" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
       <c r="I48" s="35" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
     </row>
     <row r="49" spans="2:9" ht="29.25" customHeight="1">
@@ -37147,19 +37251,19 @@
         <v>3</v>
       </c>
       <c r="E49" s="42" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
       <c r="G49" s="36" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
       <c r="H49" s="38" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="I49" s="36" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
     </row>
     <row r="50" spans="2:9" ht="28.5" customHeight="1">
@@ -37169,19 +37273,19 @@
         <v>4</v>
       </c>
       <c r="E50" s="42" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
       <c r="G50" s="36" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
       <c r="H50" s="36" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="I50" s="36" t="s">
-        <v>284</v>
+        <v>294</v>
       </c>
     </row>
     <row r="51" spans="2:9" ht="32.25" customHeight="1">
@@ -37191,13 +37295,13 @@
         <v>5</v>
       </c>
       <c r="E51" s="40" t="s">
-        <v>285</v>
+        <v>295</v>
       </c>
       <c r="F51" s="40" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="G51" s="42" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="H51" s="40"/>
       <c r="I51" s="40"/>
@@ -37263,54 +37367,54 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="15">
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
+      <c r="B2" s="114"/>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
     </row>
     <row r="3" spans="1:11" ht="15">
       <c r="B3" s="111" t="s">
-        <v>158</v>
-      </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
+        <v>168</v>
+      </c>
+      <c r="C3" s="115"/>
+      <c r="D3" s="115"/>
+      <c r="E3" s="115"/>
+      <c r="F3" s="115"/>
+      <c r="G3" s="115"/>
+      <c r="H3" s="115"/>
+      <c r="I3" s="115"/>
+      <c r="J3" s="115"/>
       <c r="K3" s="33"/>
     </row>
     <row r="4" spans="1:11">
       <c r="B4" s="32" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="E4" s="34" t="s">
         <v>5</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>291</v>
+        <v>301</v>
       </c>
       <c r="I4" s="34" t="s">
-        <v>292</v>
+        <v>302</v>
       </c>
       <c r="J4" s="34" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="33" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -37319,28 +37423,28 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="D5" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="E5" t="s">
-        <v>296</v>
+        <v>306</v>
       </c>
       <c r="F5" t="s">
-        <v>297</v>
+        <v>307</v>
       </c>
       <c r="G5">
         <v>9876543567</v>
       </c>
       <c r="H5" s="75" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="I5" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="J5" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="K5" s="27">
         <v>1</v>
@@ -37352,28 +37456,28 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="D6" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="E6" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="F6" t="s">
-        <v>304</v>
+        <v>314</v>
       </c>
       <c r="G6">
         <v>9876873567</v>
       </c>
       <c r="H6" s="75" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="I6" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="J6" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="K6" s="27">
         <v>2</v>
@@ -37384,28 +37488,28 @@
         <v>3</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="D7" s="29" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>307</v>
+        <v>317</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>308</v>
+        <v>318</v>
       </c>
       <c r="G7" s="29">
         <v>8975908765</v>
       </c>
       <c r="H7" s="74" t="s">
+        <v>319</v>
+      </c>
+      <c r="I7" s="29" t="s">
         <v>309</v>
       </c>
-      <c r="I7" s="29" t="s">
-        <v>299</v>
-      </c>
       <c r="J7" s="29" t="s">
-        <v>300</v>
+        <v>310</v>
       </c>
       <c r="K7" s="30">
         <v>1</v>
@@ -37417,108 +37521,108 @@
       <c r="F9" s="31"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="B10" s="105" t="s">
-        <v>310</v>
-      </c>
-      <c r="C10" s="107"/>
-      <c r="E10" s="105" t="s">
-        <v>311</v>
-      </c>
-      <c r="F10" s="107"/>
-      <c r="H10" s="105" t="s">
-        <v>312</v>
-      </c>
-      <c r="I10" s="107"/>
+      <c r="B10" s="102" t="s">
+        <v>320</v>
+      </c>
+      <c r="C10" s="103"/>
+      <c r="E10" s="102" t="s">
+        <v>321</v>
+      </c>
+      <c r="F10" s="103"/>
+      <c r="H10" s="102" t="s">
+        <v>322</v>
+      </c>
+      <c r="I10" s="103"/>
     </row>
     <row r="11" spans="1:11" ht="15">
       <c r="B11" s="76" t="s">
-        <v>293</v>
+        <v>303</v>
       </c>
       <c r="C11" s="77" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="32" t="s">
-        <v>287</v>
+        <v>297</v>
       </c>
       <c r="F11" s="79" t="s">
-        <v>314</v>
+        <v>324</v>
       </c>
       <c r="G11" s="72"/>
       <c r="H11" s="32" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="I11" s="79" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
       <c r="J11" s="72"/>
     </row>
     <row r="12" spans="1:11">
       <c r="B12" s="26" t="s">
-        <v>316</v>
+        <v>326</v>
       </c>
       <c r="C12" s="27" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>318</v>
+        <v>328</v>
       </c>
       <c r="H12" s="26" t="s">
-        <v>295</v>
+        <v>305</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15">
       <c r="B13" s="28" t="s">
-        <v>320</v>
+        <v>330</v>
       </c>
       <c r="C13" s="30" t="s">
-        <v>321</v>
+        <v>331</v>
       </c>
       <c r="E13" s="78" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="H13" s="28" t="s">
-        <v>302</v>
+        <v>312</v>
       </c>
       <c r="I13" s="30" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="15">
-      <c r="B19" s="105" t="s">
-        <v>324</v>
-      </c>
-      <c r="C19" s="106"/>
-      <c r="D19" s="106"/>
-      <c r="E19" s="107"/>
+      <c r="B19" s="102" t="s">
+        <v>334</v>
+      </c>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
+      <c r="E19" s="103"/>
       <c r="F19" s="31"/>
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="32" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>326</v>
+        <v>336</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="15">
       <c r="B21" s="81" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -37527,12 +37631,12 @@
         <v>37237</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="15">
       <c r="B22" s="78" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="C22" s="82">
         <v>2</v>
@@ -37541,7 +37645,7 @@
         <v>36903</v>
       </c>
       <c r="E22" s="84" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
     </row>
     <row r="24" spans="2:9">
@@ -37555,34 +37659,34 @@
     </row>
     <row r="28" spans="2:9" ht="15">
       <c r="B28" s="108" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="C28" s="109"/>
       <c r="D28" s="109"/>
       <c r="E28" s="109"/>
       <c r="F28" s="109"/>
       <c r="G28" s="110"/>
-      <c r="H28" s="120"/>
-      <c r="I28" s="120"/>
+      <c r="H28" s="113"/>
+      <c r="I28" s="113"/>
     </row>
     <row r="29" spans="2:9">
       <c r="B29" s="32" t="s">
-        <v>332</v>
+        <v>342</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="E29" s="34" t="s">
-        <v>334</v>
+        <v>344</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>335</v>
+        <v>345</v>
       </c>
       <c r="G29" s="33" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
     </row>
     <row r="30" spans="2:9">
@@ -37590,7 +37694,7 @@
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -37608,7 +37712,7 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -37626,7 +37730,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="D32" s="29">
         <v>1</v>
@@ -37644,7 +37748,7 @@
     </row>
     <row r="36" spans="2:8" ht="15">
       <c r="B36" s="108" t="s">
-        <v>337</v>
+        <v>347</v>
       </c>
       <c r="C36" s="109"/>
       <c r="D36" s="109"/>
@@ -37655,25 +37759,25 @@
     </row>
     <row r="37" spans="2:8">
       <c r="B37" s="32" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C37" s="34" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="D37" s="34" t="s">
-        <v>339</v>
+        <v>349</v>
       </c>
       <c r="E37" s="34" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="F37" s="34" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="G37" s="34" t="s">
-        <v>342</v>
+        <v>352</v>
       </c>
       <c r="H37" s="33" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
     </row>
     <row r="38" spans="2:8">
@@ -37681,13 +37785,13 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="D38" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="E38" t="s">
-        <v>343</v>
+        <v>353</v>
       </c>
       <c r="F38">
         <v>2019</v>
@@ -37702,13 +37806,13 @@
         <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="D39" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
       <c r="E39" t="s">
-        <v>345</v>
+        <v>355</v>
       </c>
       <c r="F39">
         <v>2020</v>
@@ -37729,28 +37833,28 @@
     </row>
     <row r="42" spans="2:8" ht="15">
       <c r="B42" s="111" t="s">
-        <v>346</v>
-      </c>
-      <c r="C42" s="112"/>
-      <c r="D42" s="112"/>
-      <c r="E42" s="112"/>
-      <c r="F42" s="113"/>
+        <v>356</v>
+      </c>
+      <c r="C42" s="115"/>
+      <c r="D42" s="115"/>
+      <c r="E42" s="115"/>
+      <c r="F42" s="112"/>
     </row>
     <row r="43" spans="2:8">
       <c r="B43" s="32" t="s">
-        <v>347</v>
+        <v>357</v>
       </c>
       <c r="C43" s="34" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="D43" s="34" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
       <c r="E43" s="34" t="s">
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="F43" s="33" t="s">
-        <v>336</v>
+        <v>346</v>
       </c>
     </row>
     <row r="44" spans="2:8">
@@ -37758,10 +37862,10 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="D44" t="s">
-        <v>350</v>
+        <v>360</v>
       </c>
       <c r="F44" s="27"/>
     </row>
@@ -37770,10 +37874,10 @@
         <v>2</v>
       </c>
       <c r="C45" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="D45" t="s">
-        <v>351</v>
+        <v>361</v>
       </c>
       <c r="F45" s="27"/>
     </row>
@@ -37782,52 +37886,52 @@
         <v>3</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="D46" s="29" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="E46" s="29"/>
       <c r="F46" s="30"/>
     </row>
     <row r="49" spans="2:22">
-      <c r="B49" s="105" t="s">
-        <v>353</v>
-      </c>
-      <c r="C49" s="106"/>
-      <c r="D49" s="106"/>
-      <c r="E49" s="106"/>
-      <c r="F49" s="106"/>
-      <c r="G49" s="106"/>
-      <c r="H49" s="107"/>
+      <c r="B49" s="102" t="s">
+        <v>363</v>
+      </c>
+      <c r="C49" s="104"/>
+      <c r="D49" s="104"/>
+      <c r="E49" s="104"/>
+      <c r="F49" s="104"/>
+      <c r="G49" s="104"/>
+      <c r="H49" s="103"/>
     </row>
     <row r="50" spans="2:22" ht="15">
       <c r="B50" s="89" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="C50" s="85" t="s">
-        <v>354</v>
+        <v>364</v>
       </c>
       <c r="D50" s="85" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="E50" s="85" t="s">
-        <v>356</v>
+        <v>366</v>
       </c>
       <c r="F50" s="34" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="G50" s="34" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="H50" s="79" t="s">
-        <v>359</v>
+        <v>369</v>
       </c>
       <c r="I50" s="72"/>
       <c r="K50" s="111" t="s">
         <v>10</v>
       </c>
-      <c r="L50" s="113"/>
+      <c r="L50" s="112"/>
       <c r="M50" s="72"/>
       <c r="R50" s="72"/>
       <c r="S50" s="72"/>
@@ -37837,19 +37941,19 @@
     </row>
     <row r="51" spans="2:22">
       <c r="B51" s="26" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="C51" t="s">
-        <v>361</v>
+        <v>371</v>
       </c>
       <c r="D51" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="E51" t="s">
-        <v>363</v>
+        <v>373</v>
       </c>
       <c r="F51" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="G51" s="80">
         <v>42370</v>
@@ -37858,27 +37962,27 @@
         <v>44562</v>
       </c>
       <c r="K51" s="32" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
       <c r="L51" s="33" t="s">
-        <v>365</v>
+        <v>375</v>
       </c>
     </row>
     <row r="52" spans="2:22">
       <c r="B52" s="26" t="s">
-        <v>360</v>
+        <v>370</v>
       </c>
       <c r="C52" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="D52" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="E52" t="s">
-        <v>368</v>
+        <v>378</v>
       </c>
       <c r="F52" s="86" t="s">
-        <v>364</v>
+        <v>374</v>
       </c>
       <c r="G52" s="80">
         <v>44562</v>
@@ -37887,10 +37991,10 @@
         <v>46023</v>
       </c>
       <c r="K52" s="26" t="s">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="L52" s="27" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
     </row>
     <row r="53" spans="2:22">
@@ -37902,62 +38006,62 @@
       <c r="G53" s="29"/>
       <c r="H53" s="30"/>
       <c r="K53" s="28" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="L53" s="30" t="s">
-        <v>370</v>
+        <v>380</v>
       </c>
     </row>
     <row r="54" spans="2:22">
       <c r="F54" s="86"/>
     </row>
     <row r="56" spans="2:22">
-      <c r="B56" s="105" t="s">
+      <c r="B56" s="102" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="106"/>
-      <c r="D56" s="106"/>
-      <c r="E56" s="106"/>
-      <c r="F56" s="106"/>
-      <c r="G56" s="106"/>
-      <c r="H56" s="106"/>
-      <c r="I56" s="107"/>
+      <c r="C56" s="104"/>
+      <c r="D56" s="104"/>
+      <c r="E56" s="104"/>
+      <c r="F56" s="104"/>
+      <c r="G56" s="104"/>
+      <c r="H56" s="104"/>
+      <c r="I56" s="103"/>
     </row>
     <row r="57" spans="2:22">
       <c r="B57" s="32" t="s">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="C57" s="34" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="D57" s="34" t="s">
-        <v>372</v>
+        <v>382</v>
       </c>
       <c r="E57" s="34" t="s">
-        <v>373</v>
+        <v>383</v>
       </c>
       <c r="F57" s="34" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="G57" s="34" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="H57" s="34" t="s">
-        <v>374</v>
+        <v>384</v>
       </c>
       <c r="I57" s="33" t="s">
-        <v>312</v>
+        <v>322</v>
       </c>
     </row>
     <row r="58" spans="2:22">
       <c r="B58" s="26" t="s">
-        <v>375</v>
+        <v>385</v>
       </c>
       <c r="C58" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="D58" t="s">
-        <v>376</v>
+        <v>386</v>
       </c>
       <c r="E58" s="80">
         <v>43466</v>
@@ -37972,18 +38076,18 @@
         <v>43466</v>
       </c>
       <c r="I58" s="27" t="s">
-        <v>319</v>
+        <v>329</v>
       </c>
     </row>
     <row r="59" spans="2:22">
       <c r="B59" s="28" t="s">
-        <v>377</v>
+        <v>387</v>
       </c>
       <c r="C59" s="29" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="E59" s="90">
         <v>43474</v>
@@ -37998,7 +38102,7 @@
         <v>43831</v>
       </c>
       <c r="I59" s="30" t="s">
-        <v>323</v>
+        <v>333</v>
       </c>
     </row>
     <row r="62" spans="2:22" ht="15">
@@ -38012,156 +38116,156 @@
       <c r="L62" s="72"/>
     </row>
     <row r="66" spans="2:11">
-      <c r="B66" s="105" t="s">
+      <c r="B66" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="C66" s="106"/>
-      <c r="D66" s="107"/>
-      <c r="F66" s="105" t="s">
+      <c r="C66" s="104"/>
+      <c r="D66" s="103"/>
+      <c r="F66" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="G66" s="106"/>
-      <c r="H66" s="107"/>
-      <c r="J66" s="105" t="s">
+      <c r="G66" s="104"/>
+      <c r="H66" s="103"/>
+      <c r="J66" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="K66" s="107"/>
+      <c r="K66" s="103"/>
     </row>
     <row r="67" spans="2:11">
       <c r="B67" s="32" t="s">
-        <v>379</v>
+        <v>389</v>
       </c>
       <c r="C67" s="34" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="D67" s="33" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="F67" s="32" t="s">
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="G67" s="34" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="H67" s="33" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="J67" s="32" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="K67" s="33" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
     </row>
     <row r="68" spans="2:11">
       <c r="B68" s="26" t="s">
-        <v>384</v>
+        <v>394</v>
       </c>
       <c r="C68" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="D68" s="27" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="F68" s="93" t="s">
-        <v>385</v>
+        <v>395</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="H68" s="94" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="J68" s="26" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="K68" s="27" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
     </row>
     <row r="69" spans="2:11" ht="15">
       <c r="B69" s="91" t="s">
-        <v>389</v>
+        <v>399</v>
       </c>
       <c r="C69" s="92" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="D69" s="30" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="F69" s="91" t="s">
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="G69" s="92" t="s">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="H69" s="95" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="J69" s="28" t="s">
-        <v>391</v>
+        <v>401</v>
       </c>
       <c r="K69" s="30" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
     </row>
     <row r="74" spans="2:11">
-      <c r="B74" s="114" t="s">
-        <v>393</v>
-      </c>
-      <c r="C74" s="115"/>
-      <c r="D74" s="116"/>
-      <c r="F74" s="117" t="s">
-        <v>394</v>
-      </c>
-      <c r="G74" s="117"/>
+      <c r="B74" s="116" t="s">
+        <v>403</v>
+      </c>
+      <c r="C74" s="117"/>
+      <c r="D74" s="118"/>
+      <c r="F74" s="119" t="s">
+        <v>404</v>
+      </c>
+      <c r="G74" s="119"/>
     </row>
     <row r="75" spans="2:11">
       <c r="B75" s="96" t="s">
-        <v>395</v>
+        <v>405</v>
       </c>
       <c r="C75" s="97" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="D75" s="98" t="s">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c r="F75" s="15" t="s">
-        <v>396</v>
+        <v>406</v>
       </c>
       <c r="G75" s="15" t="s">
-        <v>394</v>
+        <v>404</v>
       </c>
     </row>
     <row r="76" spans="2:11" ht="15">
       <c r="B76" s="99" t="s">
-        <v>397</v>
+        <v>407</v>
       </c>
       <c r="C76" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="D76" s="100" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="F76" s="99" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
       <c r="G76" s="100" t="s">
-        <v>399</v>
+        <v>409</v>
       </c>
     </row>
     <row r="77" spans="2:11" ht="15">
       <c r="B77" s="26" t="s">
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="C77" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="D77" s="27" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="F77" s="101" t="s">
-        <v>401</v>
+        <v>411</v>
       </c>
       <c r="G77" s="30" t="s">
         <v>23</v>
@@ -38169,53 +38273,53 @@
     </row>
     <row r="78" spans="2:11">
       <c r="B78" s="26" t="s">
-        <v>402</v>
+        <v>412</v>
       </c>
       <c r="C78" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="D78" s="27" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
     </row>
     <row r="79" spans="2:11">
       <c r="B79" s="28" t="s">
-        <v>403</v>
+        <v>413</v>
       </c>
       <c r="C79" s="29" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="D79" s="30" t="s">
-        <v>398</v>
+        <v>408</v>
       </c>
     </row>
     <row r="84" spans="2:9">
-      <c r="B84" s="102" t="s">
-        <v>404</v>
-      </c>
-      <c r="C84" s="103"/>
-      <c r="D84" s="104"/>
+      <c r="B84" s="105" t="s">
+        <v>414</v>
+      </c>
+      <c r="C84" s="106"/>
+      <c r="D84" s="107"/>
     </row>
     <row r="85" spans="2:9">
       <c r="B85" s="28" t="s">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="C85" s="29" t="s">
-        <v>325</v>
+        <v>335</v>
       </c>
       <c r="D85" s="30" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
     </row>
     <row r="86" spans="2:9">
       <c r="C86" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
     </row>
     <row r="87" spans="2:9" ht="15">
       <c r="B87" s="72"/>
       <c r="C87" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
       <c r="E87" s="72"/>
       <c r="F87" s="72"/>
@@ -38224,7 +38328,7 @@
     </row>
     <row r="88" spans="2:9">
       <c r="C88" t="s">
-        <v>408</v>
+        <v>418</v>
       </c>
     </row>
     <row r="96" spans="2:9" ht="15">
@@ -38234,17 +38338,17 @@
       <c r="B105" s="72"/>
     </row>
     <row r="115" spans="2:3" ht="15">
-      <c r="B115" s="118" t="s">
-        <v>409</v>
-      </c>
-      <c r="C115" s="119"/>
+      <c r="B115" s="120" t="s">
+        <v>419</v>
+      </c>
+      <c r="C115" s="121"/>
     </row>
     <row r="116" spans="2:3">
       <c r="B116" s="32" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
       <c r="C116" s="33" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
     </row>
     <row r="117" spans="2:3">
@@ -38272,21 +38376,21 @@
   </sheetData>
   <mergeCells count="20">
     <mergeCell ref="B115:C115"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="F66:H66"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="F66:H66"/>
     <mergeCell ref="J66:K66"/>
     <mergeCell ref="B19:E19"/>
     <mergeCell ref="B49:H49"/>
     <mergeCell ref="B84:D84"/>
     <mergeCell ref="B56:I56"/>
     <mergeCell ref="B36:H36"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="H28:I28"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="B42:F42"/>
     <mergeCell ref="B74:D74"/>
@@ -38305,7 +38409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D3CFBF-880F-481E-9D27-6F5C85AAC27F}">
   <dimension ref="V29:Y48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="Y48" sqref="Y48"/>
     </sheetView>
   </sheetViews>
@@ -38313,7 +38417,7 @@
   <sheetData>
     <row r="29" spans="22:22">
       <c r="V29" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
     </row>
     <row r="48" spans="25:25">
@@ -38352,28 +38456,28 @@
   <sheetData>
     <row r="1" spans="3:10" ht="23.25">
       <c r="J1" s="12" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="3:10" ht="20.25">
       <c r="C4" s="11" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="D4" s="6"/>
     </row>
     <row r="6" spans="3:10" ht="20.25">
       <c r="D6" s="10" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
     </row>
     <row r="21" spans="4:4" ht="20.25">
       <c r="D21" s="10" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
     </row>
     <row r="33" spans="4:8" ht="20.25">
       <c r="D33" s="13" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
     </row>
     <row r="38" spans="4:8">
@@ -38381,34 +38485,34 @@
     </row>
     <row r="46" spans="4:8" ht="20.25">
       <c r="D46" s="10" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
     </row>
     <row r="59" spans="3:4" ht="20.25">
       <c r="C59" s="11" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="D59" s="10"/>
     </row>
     <row r="61" spans="3:4" ht="20.25">
       <c r="D61" s="10" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
     </row>
     <row r="74" spans="4:5" ht="20.25">
       <c r="D74" s="10" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
       <c r="E74" s="10"/>
     </row>
     <row r="85" spans="4:4" ht="20.25">
       <c r="D85" s="10" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
     </row>
     <row r="296" spans="3:5" ht="18">
       <c r="C296" s="9" t="s">
-        <v>419</v>
+        <v>429</v>
       </c>
       <c r="D296" s="9"/>
       <c r="E296" s="9"/>
@@ -38445,10 +38549,10 @@
     <row r="1" spans="1:3">
       <c r="A1" s="17"/>
       <c r="B1" s="18" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -38458,47 +38562,47 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="15" t="s">
-        <v>420</v>
+        <v>430</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>421</v>
+        <v>431</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>422</v>
+        <v>432</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="15"/>
       <c r="B4" s="16" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="15"/>
       <c r="B5" s="16" t="s">
-        <v>424</v>
+        <v>434</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>424</v>
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="15"/>
       <c r="B6" s="16" t="s">
-        <v>425</v>
+        <v>435</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>426</v>
+        <v>436</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="15"/>
       <c r="B7" s="16"/>
       <c r="C7" s="15" t="s">
-        <v>427</v>
+        <v>437</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -38553,10 +38657,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="15" t="s">
-        <v>428</v>
+        <v>438</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>422</v>
+        <v>432</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>4</v>
@@ -38565,31 +38669,31 @@
     <row r="19" spans="1:4">
       <c r="A19" s="15"/>
       <c r="B19" s="16" t="s">
-        <v>429</v>
+        <v>439</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>429</v>
+        <v>439</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="15"/>
       <c r="B20" s="16" t="s">
-        <v>430</v>
+        <v>440</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>430</v>
+        <v>440</v>
       </c>
       <c r="D20" t="s">
-        <v>431</v>
+        <v>441</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="15"/>
       <c r="B21" s="16" t="s">
-        <v>432</v>
+        <v>442</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>432</v>
+        <v>442</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -38623,128 +38727,128 @@
   <sheetData>
     <row r="3" spans="1:15" ht="20.25">
       <c r="L3" s="10" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>434</v>
+        <v>444</v>
       </c>
     </row>
     <row r="9" spans="1:15">
       <c r="A9" t="s">
-        <v>435</v>
+        <v>445</v>
       </c>
       <c r="B9" t="s">
-        <v>434</v>
+        <v>444</v>
       </c>
       <c r="O9" t="s">
-        <v>436</v>
+        <v>446</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>437</v>
+        <v>447</v>
       </c>
       <c r="B11" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
     </row>
     <row r="13" spans="1:15">
       <c r="A13" t="s">
-        <v>439</v>
+        <v>449</v>
       </c>
       <c r="B13" t="s">
-        <v>440</v>
+        <v>450</v>
       </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
-        <v>441</v>
+        <v>451</v>
       </c>
       <c r="B15" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
-        <v>443</v>
+        <v>453</v>
       </c>
       <c r="B17" t="s">
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="O17" t="s">
-        <v>445</v>
+        <v>455</v>
       </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="B19" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
     </row>
     <row r="21" spans="1:15">
       <c r="A21" t="s">
-        <v>448</v>
+        <v>458</v>
       </c>
       <c r="B21" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>450</v>
+        <v>460</v>
       </c>
       <c r="B23" t="s">
-        <v>451</v>
+        <v>461</v>
       </c>
     </row>
     <row r="25" spans="1:15">
       <c r="A25" t="s">
-        <v>452</v>
+        <v>462</v>
       </c>
       <c r="B25" t="s">
-        <v>453</v>
+        <v>463</v>
       </c>
       <c r="O25" t="s">
-        <v>454</v>
+        <v>464</v>
       </c>
     </row>
     <row r="32" spans="1:15">
       <c r="O32" t="s">
-        <v>455</v>
+        <v>465</v>
       </c>
     </row>
     <row r="39" spans="15:15">
       <c r="O39" s="20" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
     </row>
     <row r="47" spans="15:15">
       <c r="O47" s="20" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
     </row>
     <row r="55" spans="15:15">
       <c r="O55" s="20" t="s">
-        <v>458</v>
+        <v>468</v>
       </c>
     </row>
     <row r="63" spans="15:15">
       <c r="O63" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
     </row>
     <row r="71" spans="15:15">
       <c r="O71" t="s">
-        <v>460</v>
+        <v>470</v>
       </c>
     </row>
     <row r="79" spans="15:15">
       <c r="O79" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>